<commit_message>
update syvbt with 2021 number of psgr airplanes
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SYVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\SYVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D544DCF-5C7D-42FD-B02A-C74F14151A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6398DF69-7AD1-4712-84EF-0D99F45EA4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -7350,37 +7350,19 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -7395,17 +7377,35 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="146">
@@ -7556,42 +7556,7 @@
     <cellStyle name="Wrap Bold" xfId="140" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
     <cellStyle name="Wrap Title" xfId="141" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -7990,8 +7955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8830,7 +8795,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8952,8 +8917,8 @@
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <f>INDEX('AEO 2021 48'!$70:$70,MATCH(About!$B$88,'AEO 2021 48'!$1:$1,0))</f>
-        <v>2120.6909179999998</v>
+        <f>INDEX('AEO 2021 48'!$70:$70,MATCH(2021,'AEO 2021 48'!$1:$1,0))</f>
+        <v>5561.7944340000004</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
@@ -9119,7 +9084,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15520,41 +15485,41 @@
     </row>
     <row r="86" spans="1:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="87" spans="1:34" ht="15" customHeight="1">
-      <c r="B87" s="80" t="s">
+      <c r="B87" s="82" t="s">
         <v>1018</v>
       </c>
-      <c r="C87" s="80"/>
-      <c r="D87" s="80"/>
-      <c r="E87" s="80"/>
-      <c r="F87" s="80"/>
-      <c r="G87" s="80"/>
-      <c r="H87" s="80"/>
-      <c r="I87" s="80"/>
-      <c r="J87" s="80"/>
-      <c r="K87" s="80"/>
-      <c r="L87" s="80"/>
-      <c r="M87" s="80"/>
-      <c r="N87" s="80"/>
-      <c r="O87" s="80"/>
-      <c r="P87" s="80"/>
-      <c r="Q87" s="80"/>
-      <c r="R87" s="80"/>
-      <c r="S87" s="80"/>
-      <c r="T87" s="80"/>
-      <c r="U87" s="80"/>
-      <c r="V87" s="80"/>
-      <c r="W87" s="80"/>
-      <c r="X87" s="80"/>
-      <c r="Y87" s="80"/>
-      <c r="Z87" s="80"/>
-      <c r="AA87" s="80"/>
-      <c r="AB87" s="80"/>
-      <c r="AC87" s="80"/>
-      <c r="AD87" s="80"/>
-      <c r="AE87" s="80"/>
-      <c r="AF87" s="80"/>
-      <c r="AG87" s="80"/>
-      <c r="AH87" s="80"/>
+      <c r="C87" s="82"/>
+      <c r="D87" s="82"/>
+      <c r="E87" s="82"/>
+      <c r="F87" s="82"/>
+      <c r="G87" s="82"/>
+      <c r="H87" s="82"/>
+      <c r="I87" s="82"/>
+      <c r="J87" s="82"/>
+      <c r="K87" s="82"/>
+      <c r="L87" s="82"/>
+      <c r="M87" s="82"/>
+      <c r="N87" s="82"/>
+      <c r="O87" s="82"/>
+      <c r="P87" s="82"/>
+      <c r="Q87" s="82"/>
+      <c r="R87" s="82"/>
+      <c r="S87" s="82"/>
+      <c r="T87" s="82"/>
+      <c r="U87" s="82"/>
+      <c r="V87" s="82"/>
+      <c r="W87" s="82"/>
+      <c r="X87" s="82"/>
+      <c r="Y87" s="82"/>
+      <c r="Z87" s="82"/>
+      <c r="AA87" s="82"/>
+      <c r="AB87" s="82"/>
+      <c r="AC87" s="82"/>
+      <c r="AD87" s="82"/>
+      <c r="AE87" s="82"/>
+      <c r="AF87" s="82"/>
+      <c r="AG87" s="82"/>
+      <c r="AH87" s="82"/>
     </row>
     <row r="88" spans="1:34" ht="15" customHeight="1">
       <c r="B88" s="18" t="s">
@@ -35997,8 +35962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK191"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="AE76" sqref="AE76"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -79250,47 +79215,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97"/>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
-      <c r="AC1" s="97"/>
-      <c r="AD1" s="97"/>
-      <c r="AE1" s="97"/>
-      <c r="AF1" s="97"/>
-      <c r="AG1" s="97"/>
-      <c r="AH1" s="97"/>
-      <c r="AI1" s="97"/>
-      <c r="AJ1" s="97"/>
-      <c r="AK1" s="97"/>
-      <c r="AL1" s="97"/>
-      <c r="AM1" s="97"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
+      <c r="AM1" s="80"/>
     </row>
     <row r="2" spans="1:43" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="36"/>
@@ -82355,7 +82320,7 @@
       <c r="AB29" s="43">
         <v>31906</v>
       </c>
-      <c r="AC29" s="98">
+      <c r="AC29" s="81">
         <v>32454</v>
       </c>
       <c r="AD29" s="47">
@@ -82370,7 +82335,7 @@
       <c r="AG29" s="43">
         <v>32819</v>
       </c>
-      <c r="AH29" s="98">
+      <c r="AH29" s="81">
         <v>33472</v>
       </c>
       <c r="AI29" s="43">
@@ -82382,7 +82347,7 @@
       <c r="AK29" s="43">
         <v>33600</v>
       </c>
-      <c r="AL29" s="98">
+      <c r="AL29" s="81">
         <v>34209</v>
       </c>
       <c r="AM29" s="43">
@@ -82477,7 +82442,7 @@
       <c r="AB30" s="43">
         <v>10775</v>
       </c>
-      <c r="AC30" s="98">
+      <c r="AC30" s="81">
         <v>10702</v>
       </c>
       <c r="AD30" s="43">
@@ -82492,7 +82457,7 @@
       <c r="AG30" s="43">
         <v>10108</v>
       </c>
-      <c r="AH30" s="98">
+      <c r="AH30" s="81">
         <v>10068</v>
       </c>
       <c r="AI30" s="43">
@@ -82504,7 +82469,7 @@
       <c r="AK30" s="43">
         <v>10152</v>
       </c>
-      <c r="AL30" s="98">
+      <c r="AL30" s="81">
         <v>10339</v>
       </c>
       <c r="AM30" s="43">
@@ -82759,30 +82724,30 @@
       </c>
     </row>
     <row r="33" spans="1:39" s="12" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A33" s="92" t="s">
+      <c r="A33" s="86" t="s">
         <v>1599</v>
       </c>
-      <c r="B33" s="92"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="92"/>
-      <c r="F33" s="92"/>
-      <c r="G33" s="92"/>
-      <c r="H33" s="92"/>
-      <c r="I33" s="92"/>
-      <c r="J33" s="92"/>
-      <c r="K33" s="92"/>
-      <c r="L33" s="92"/>
-      <c r="M33" s="92"/>
-      <c r="N33" s="92"/>
-      <c r="O33" s="92"/>
-      <c r="P33" s="92"/>
-      <c r="Q33" s="92"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
-      <c r="V33" s="92"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="86"/>
+      <c r="P33" s="86"/>
+      <c r="Q33" s="86"/>
+      <c r="R33" s="86"/>
+      <c r="S33" s="86"/>
+      <c r="T33" s="86"/>
+      <c r="U33" s="86"/>
+      <c r="V33" s="86"/>
       <c r="W33" s="53"/>
       <c r="X33" s="53"/>
       <c r="Y33" s="53"/>
@@ -82795,56 +82760,56 @@
       <c r="AM33" s="7"/>
     </row>
     <row r="34" spans="1:39" s="12" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A34" s="93"/>
-      <c r="B34" s="93"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="93"/>
-      <c r="P34" s="93"/>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="93"/>
-      <c r="S34" s="93"/>
-      <c r="T34" s="93"/>
-      <c r="U34" s="93"/>
-      <c r="V34" s="93"/>
+      <c r="A34" s="87"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="87"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
+      <c r="M34" s="87"/>
+      <c r="N34" s="87"/>
+      <c r="O34" s="87"/>
+      <c r="P34" s="87"/>
+      <c r="Q34" s="87"/>
+      <c r="R34" s="87"/>
+      <c r="S34" s="87"/>
+      <c r="T34" s="87"/>
+      <c r="U34" s="87"/>
+      <c r="V34" s="87"/>
       <c r="AL34" s="7"/>
       <c r="AM34" s="7"/>
     </row>
     <row r="35" spans="1:39" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="94" t="s">
+      <c r="A35" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="94"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="94"/>
-      <c r="J35" s="94"/>
-      <c r="K35" s="94"/>
-      <c r="L35" s="94"/>
-      <c r="M35" s="94"/>
-      <c r="N35" s="94"/>
-      <c r="O35" s="94"/>
-      <c r="P35" s="94"/>
-      <c r="Q35" s="94"/>
-      <c r="R35" s="94"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="94"/>
-      <c r="V35" s="94"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="88"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="88"/>
+      <c r="N35" s="88"/>
+      <c r="O35" s="88"/>
+      <c r="P35" s="88"/>
+      <c r="Q35" s="88"/>
+      <c r="R35" s="88"/>
+      <c r="S35" s="88"/>
+      <c r="T35" s="88"/>
+      <c r="U35" s="88"/>
+      <c r="V35" s="88"/>
       <c r="W35" s="79"/>
       <c r="X35" s="79"/>
       <c r="Y35" s="79"/>
@@ -82864,30 +82829,30 @@
       <c r="AM35" s="7"/>
     </row>
     <row r="36" spans="1:39" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A36" s="87" t="s">
+      <c r="A36" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="87"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="87"/>
-      <c r="I36" s="87"/>
-      <c r="J36" s="87"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
-      <c r="M36" s="87"/>
-      <c r="N36" s="87"/>
-      <c r="O36" s="87"/>
-      <c r="P36" s="87"/>
-      <c r="Q36" s="87"/>
-      <c r="R36" s="87"/>
-      <c r="S36" s="87"/>
-      <c r="T36" s="87"/>
-      <c r="U36" s="87"/>
-      <c r="V36" s="87"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89"/>
+      <c r="Q36" s="89"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="89"/>
+      <c r="U36" s="89"/>
+      <c r="V36" s="89"/>
       <c r="W36" s="79"/>
       <c r="X36" s="79"/>
       <c r="Y36" s="79"/>
@@ -82907,30 +82872,30 @@
       <c r="AM36" s="7"/>
     </row>
     <row r="37" spans="1:39" s="14" customFormat="1" ht="38.85" customHeight="1">
-      <c r="A37" s="95" t="s">
+      <c r="A37" s="90" t="s">
         <v>974</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="95"/>
-      <c r="J37" s="95"/>
-      <c r="K37" s="95"/>
-      <c r="L37" s="95"/>
-      <c r="M37" s="95"/>
-      <c r="N37" s="95"/>
-      <c r="O37" s="95"/>
-      <c r="P37" s="95"/>
-      <c r="Q37" s="95"/>
-      <c r="R37" s="95"/>
-      <c r="S37" s="95"/>
-      <c r="T37" s="95"/>
-      <c r="U37" s="95"/>
-      <c r="V37" s="95"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="90"/>
+      <c r="L37" s="90"/>
+      <c r="M37" s="90"/>
+      <c r="N37" s="90"/>
+      <c r="O37" s="90"/>
+      <c r="P37" s="90"/>
+      <c r="Q37" s="90"/>
+      <c r="R37" s="90"/>
+      <c r="S37" s="90"/>
+      <c r="T37" s="90"/>
+      <c r="U37" s="90"/>
+      <c r="V37" s="90"/>
       <c r="W37" s="79"/>
       <c r="X37" s="79"/>
       <c r="Y37" s="79"/>
@@ -82950,30 +82915,30 @@
       <c r="AM37" s="7"/>
     </row>
     <row r="38" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="89" t="s">
         <v>1600</v>
       </c>
-      <c r="B38" s="87"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
-      <c r="I38" s="87"/>
-      <c r="J38" s="87"/>
-      <c r="K38" s="87"/>
-      <c r="L38" s="87"/>
-      <c r="M38" s="87"/>
-      <c r="N38" s="87"/>
-      <c r="O38" s="87"/>
-      <c r="P38" s="87"/>
-      <c r="Q38" s="87"/>
-      <c r="R38" s="87"/>
-      <c r="S38" s="87"/>
-      <c r="T38" s="87"/>
-      <c r="U38" s="87"/>
-      <c r="V38" s="87"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89"/>
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="89"/>
+      <c r="T38" s="89"/>
+      <c r="U38" s="89"/>
+      <c r="V38" s="89"/>
       <c r="W38" s="79"/>
       <c r="X38" s="79"/>
       <c r="Y38" s="79"/>
@@ -82993,30 +82958,30 @@
       <c r="AM38" s="7"/>
     </row>
     <row r="39" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="89" t="s">
         <v>975</v>
       </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="87"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
-      <c r="H39" s="87"/>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="87"/>
-      <c r="M39" s="87"/>
-      <c r="N39" s="87"/>
-      <c r="O39" s="87"/>
-      <c r="P39" s="87"/>
-      <c r="Q39" s="87"/>
-      <c r="R39" s="87"/>
-      <c r="S39" s="87"/>
-      <c r="T39" s="87"/>
-      <c r="U39" s="87"/>
-      <c r="V39" s="87"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="89"/>
+      <c r="M39" s="89"/>
+      <c r="N39" s="89"/>
+      <c r="O39" s="89"/>
+      <c r="P39" s="89"/>
+      <c r="Q39" s="89"/>
+      <c r="R39" s="89"/>
+      <c r="S39" s="89"/>
+      <c r="T39" s="89"/>
+      <c r="U39" s="89"/>
+      <c r="V39" s="89"/>
       <c r="W39" s="79"/>
       <c r="X39" s="79"/>
       <c r="Y39" s="79"/>
@@ -83036,30 +83001,30 @@
       <c r="AM39" s="7"/>
     </row>
     <row r="40" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A40" s="87" t="s">
+      <c r="A40" s="89" t="s">
         <v>976</v>
       </c>
-      <c r="B40" s="87"/>
-      <c r="C40" s="87"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="87"/>
-      <c r="J40" s="87"/>
-      <c r="K40" s="87"/>
-      <c r="L40" s="87"/>
-      <c r="M40" s="87"/>
-      <c r="N40" s="87"/>
-      <c r="O40" s="87"/>
-      <c r="P40" s="87"/>
-      <c r="Q40" s="87"/>
-      <c r="R40" s="87"/>
-      <c r="S40" s="87"/>
-      <c r="T40" s="87"/>
-      <c r="U40" s="87"/>
-      <c r="V40" s="87"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="89"/>
+      <c r="N40" s="89"/>
+      <c r="O40" s="89"/>
+      <c r="P40" s="89"/>
+      <c r="Q40" s="89"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="89"/>
+      <c r="T40" s="89"/>
+      <c r="U40" s="89"/>
+      <c r="V40" s="89"/>
       <c r="W40" s="79"/>
       <c r="X40" s="79"/>
       <c r="Y40" s="79"/>
@@ -83079,30 +83044,30 @@
       <c r="AM40" s="7"/>
     </row>
     <row r="41" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A41" s="87" t="s">
+      <c r="A41" s="89" t="s">
         <v>977</v>
       </c>
-      <c r="B41" s="87"/>
-      <c r="C41" s="87"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="87"/>
-      <c r="I41" s="87"/>
-      <c r="J41" s="87"/>
-      <c r="K41" s="87"/>
-      <c r="L41" s="87"/>
-      <c r="M41" s="87"/>
-      <c r="N41" s="87"/>
-      <c r="O41" s="87"/>
-      <c r="P41" s="87"/>
-      <c r="Q41" s="87"/>
-      <c r="R41" s="87"/>
-      <c r="S41" s="87"/>
-      <c r="T41" s="87"/>
-      <c r="U41" s="87"/>
-      <c r="V41" s="87"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="89"/>
+      <c r="L41" s="89"/>
+      <c r="M41" s="89"/>
+      <c r="N41" s="89"/>
+      <c r="O41" s="89"/>
+      <c r="P41" s="89"/>
+      <c r="Q41" s="89"/>
+      <c r="R41" s="89"/>
+      <c r="S41" s="89"/>
+      <c r="T41" s="89"/>
+      <c r="U41" s="89"/>
+      <c r="V41" s="89"/>
       <c r="W41" s="79"/>
       <c r="X41" s="79"/>
       <c r="Y41" s="79"/>
@@ -83122,30 +83087,30 @@
       <c r="AM41" s="7"/>
     </row>
     <row r="42" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A42" s="96" t="s">
+      <c r="A42" s="91" t="s">
         <v>978</v>
       </c>
-      <c r="B42" s="96"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="96"/>
-      <c r="K42" s="96"/>
-      <c r="L42" s="96"/>
-      <c r="M42" s="96"/>
-      <c r="N42" s="96"/>
-      <c r="O42" s="96"/>
-      <c r="P42" s="96"/>
-      <c r="Q42" s="96"/>
-      <c r="R42" s="96"/>
-      <c r="S42" s="96"/>
-      <c r="T42" s="96"/>
-      <c r="U42" s="96"/>
-      <c r="V42" s="96"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="91"/>
+      <c r="M42" s="91"/>
+      <c r="N42" s="91"/>
+      <c r="O42" s="91"/>
+      <c r="P42" s="91"/>
+      <c r="Q42" s="91"/>
+      <c r="R42" s="91"/>
+      <c r="S42" s="91"/>
+      <c r="T42" s="91"/>
+      <c r="U42" s="91"/>
+      <c r="V42" s="91"/>
       <c r="W42" s="79"/>
       <c r="X42" s="79"/>
       <c r="Y42" s="79"/>
@@ -83165,30 +83130,30 @@
       <c r="AM42" s="7"/>
     </row>
     <row r="43" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="91" t="s">
         <v>979</v>
       </c>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="96"/>
-      <c r="F43" s="96"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="96"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="96"/>
-      <c r="K43" s="96"/>
-      <c r="L43" s="96"/>
-      <c r="M43" s="96"/>
-      <c r="N43" s="96"/>
-      <c r="O43" s="96"/>
-      <c r="P43" s="96"/>
-      <c r="Q43" s="96"/>
-      <c r="R43" s="96"/>
-      <c r="S43" s="96"/>
-      <c r="T43" s="96"/>
-      <c r="U43" s="96"/>
-      <c r="V43" s="96"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
+      <c r="O43" s="91"/>
+      <c r="P43" s="91"/>
+      <c r="Q43" s="91"/>
+      <c r="R43" s="91"/>
+      <c r="S43" s="91"/>
+      <c r="T43" s="91"/>
+      <c r="U43" s="91"/>
+      <c r="V43" s="91"/>
       <c r="W43" s="79"/>
       <c r="X43" s="79"/>
       <c r="Y43" s="79"/>
@@ -83208,30 +83173,30 @@
       <c r="AM43" s="7"/>
     </row>
     <row r="44" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A44" s="95" t="s">
+      <c r="A44" s="90" t="s">
         <v>980</v>
       </c>
-      <c r="B44" s="95"/>
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="95"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="95"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="95"/>
-      <c r="L44" s="95"/>
-      <c r="M44" s="95"/>
-      <c r="N44" s="95"/>
-      <c r="O44" s="95"/>
-      <c r="P44" s="95"/>
-      <c r="Q44" s="95"/>
-      <c r="R44" s="95"/>
-      <c r="S44" s="95"/>
-      <c r="T44" s="95"/>
-      <c r="U44" s="95"/>
-      <c r="V44" s="95"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="90"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="90"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="90"/>
+      <c r="L44" s="90"/>
+      <c r="M44" s="90"/>
+      <c r="N44" s="90"/>
+      <c r="O44" s="90"/>
+      <c r="P44" s="90"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="90"/>
+      <c r="S44" s="90"/>
+      <c r="T44" s="90"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="90"/>
       <c r="W44" s="79"/>
       <c r="X44" s="79"/>
       <c r="Y44" s="79"/>
@@ -83251,30 +83216,30 @@
       <c r="AM44" s="7"/>
     </row>
     <row r="45" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A45" s="87" t="s">
+      <c r="A45" s="89" t="s">
         <v>981</v>
       </c>
-      <c r="B45" s="87"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
-      <c r="F45" s="87"/>
-      <c r="G45" s="87"/>
-      <c r="H45" s="87"/>
-      <c r="I45" s="87"/>
-      <c r="J45" s="87"/>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="87"/>
-      <c r="N45" s="87"/>
-      <c r="O45" s="87"/>
-      <c r="P45" s="87"/>
-      <c r="Q45" s="87"/>
-      <c r="R45" s="87"/>
-      <c r="S45" s="87"/>
-      <c r="T45" s="87"/>
-      <c r="U45" s="87"/>
-      <c r="V45" s="87"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="89"/>
+      <c r="O45" s="89"/>
+      <c r="P45" s="89"/>
+      <c r="Q45" s="89"/>
+      <c r="R45" s="89"/>
+      <c r="S45" s="89"/>
+      <c r="T45" s="89"/>
+      <c r="U45" s="89"/>
+      <c r="V45" s="89"/>
       <c r="W45" s="79"/>
       <c r="X45" s="79"/>
       <c r="Y45" s="79"/>
@@ -83294,30 +83259,30 @@
       <c r="AM45" s="7"/>
     </row>
     <row r="46" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A46" s="87" t="s">
+      <c r="A46" s="89" t="s">
         <v>982</v>
       </c>
-      <c r="B46" s="87"/>
-      <c r="C46" s="87"/>
-      <c r="D46" s="87"/>
-      <c r="E46" s="87"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="87"/>
-      <c r="I46" s="87"/>
-      <c r="J46" s="87"/>
-      <c r="K46" s="87"/>
-      <c r="L46" s="87"/>
-      <c r="M46" s="87"/>
-      <c r="N46" s="87"/>
-      <c r="O46" s="87"/>
-      <c r="P46" s="87"/>
-      <c r="Q46" s="87"/>
-      <c r="R46" s="87"/>
-      <c r="S46" s="87"/>
-      <c r="T46" s="87"/>
-      <c r="U46" s="87"/>
-      <c r="V46" s="87"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="89"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="89"/>
+      <c r="J46" s="89"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="89"/>
+      <c r="M46" s="89"/>
+      <c r="N46" s="89"/>
+      <c r="O46" s="89"/>
+      <c r="P46" s="89"/>
+      <c r="Q46" s="89"/>
+      <c r="R46" s="89"/>
+      <c r="S46" s="89"/>
+      <c r="T46" s="89"/>
+      <c r="U46" s="89"/>
+      <c r="V46" s="89"/>
       <c r="W46" s="79"/>
       <c r="X46" s="79"/>
       <c r="Y46" s="79"/>
@@ -83337,30 +83302,30 @@
       <c r="AM46" s="7"/>
     </row>
     <row r="47" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="89" t="s">
         <v>983</v>
       </c>
-      <c r="B47" s="87"/>
-      <c r="C47" s="87"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="87"/>
-      <c r="F47" s="87"/>
-      <c r="G47" s="87"/>
-      <c r="H47" s="87"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="87"/>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
-      <c r="M47" s="87"/>
-      <c r="N47" s="87"/>
-      <c r="O47" s="87"/>
-      <c r="P47" s="87"/>
-      <c r="Q47" s="87"/>
-      <c r="R47" s="87"/>
-      <c r="S47" s="87"/>
-      <c r="T47" s="87"/>
-      <c r="U47" s="87"/>
-      <c r="V47" s="87"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
+      <c r="I47" s="89"/>
+      <c r="J47" s="89"/>
+      <c r="K47" s="89"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="89"/>
+      <c r="N47" s="89"/>
+      <c r="O47" s="89"/>
+      <c r="P47" s="89"/>
+      <c r="Q47" s="89"/>
+      <c r="R47" s="89"/>
+      <c r="S47" s="89"/>
+      <c r="T47" s="89"/>
+      <c r="U47" s="89"/>
+      <c r="V47" s="89"/>
       <c r="W47" s="79"/>
       <c r="X47" s="79"/>
       <c r="Y47" s="79"/>
@@ -83380,30 +83345,30 @@
       <c r="AM47" s="7"/>
     </row>
     <row r="48" spans="1:39" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A48" s="87" t="s">
+      <c r="A48" s="89" t="s">
         <v>984</v>
       </c>
-      <c r="B48" s="87"/>
-      <c r="C48" s="87"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="87"/>
-      <c r="I48" s="87"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="87"/>
-      <c r="M48" s="87"/>
-      <c r="N48" s="87"/>
-      <c r="O48" s="87"/>
-      <c r="P48" s="87"/>
-      <c r="Q48" s="87"/>
-      <c r="R48" s="87"/>
-      <c r="S48" s="87"/>
-      <c r="T48" s="87"/>
-      <c r="U48" s="87"/>
-      <c r="V48" s="87"/>
+      <c r="B48" s="89"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
+      <c r="H48" s="89"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="89"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="89"/>
+      <c r="N48" s="89"/>
+      <c r="O48" s="89"/>
+      <c r="P48" s="89"/>
+      <c r="Q48" s="89"/>
+      <c r="R48" s="89"/>
+      <c r="S48" s="89"/>
+      <c r="T48" s="89"/>
+      <c r="U48" s="89"/>
+      <c r="V48" s="89"/>
       <c r="W48" s="79"/>
       <c r="X48" s="79"/>
       <c r="Y48" s="79"/>
@@ -83423,30 +83388,30 @@
       <c r="AM48" s="7"/>
     </row>
     <row r="49" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A49" s="87" t="s">
+      <c r="A49" s="89" t="s">
         <v>985</v>
       </c>
-      <c r="B49" s="87"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="87"/>
-      <c r="E49" s="87"/>
-      <c r="F49" s="87"/>
-      <c r="G49" s="87"/>
-      <c r="H49" s="87"/>
-      <c r="I49" s="87"/>
-      <c r="J49" s="87"/>
-      <c r="K49" s="87"/>
-      <c r="L49" s="87"/>
-      <c r="M49" s="87"/>
-      <c r="N49" s="87"/>
-      <c r="O49" s="87"/>
-      <c r="P49" s="87"/>
-      <c r="Q49" s="87"/>
-      <c r="R49" s="87"/>
-      <c r="S49" s="87"/>
-      <c r="T49" s="87"/>
-      <c r="U49" s="87"/>
-      <c r="V49" s="87"/>
+      <c r="B49" s="89"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="89"/>
+      <c r="G49" s="89"/>
+      <c r="H49" s="89"/>
+      <c r="I49" s="89"/>
+      <c r="J49" s="89"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="89"/>
+      <c r="M49" s="89"/>
+      <c r="N49" s="89"/>
+      <c r="O49" s="89"/>
+      <c r="P49" s="89"/>
+      <c r="Q49" s="89"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="89"/>
+      <c r="T49" s="89"/>
+      <c r="U49" s="89"/>
+      <c r="V49" s="89"/>
       <c r="W49" s="79"/>
       <c r="X49" s="79"/>
       <c r="Y49" s="79"/>
@@ -83466,30 +83431,30 @@
       <c r="AM49" s="7"/>
     </row>
     <row r="50" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A50" s="87" t="s">
+      <c r="A50" s="89" t="s">
         <v>1601</v>
       </c>
-      <c r="B50" s="87"/>
-      <c r="C50" s="87"/>
-      <c r="D50" s="87"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="87"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="87"/>
-      <c r="I50" s="87"/>
-      <c r="J50" s="87"/>
-      <c r="K50" s="87"/>
-      <c r="L50" s="87"/>
-      <c r="M50" s="87"/>
-      <c r="N50" s="87"/>
-      <c r="O50" s="87"/>
-      <c r="P50" s="87"/>
-      <c r="Q50" s="87"/>
-      <c r="R50" s="87"/>
-      <c r="S50" s="87"/>
-      <c r="T50" s="87"/>
-      <c r="U50" s="87"/>
-      <c r="V50" s="87"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
+      <c r="G50" s="89"/>
+      <c r="H50" s="89"/>
+      <c r="I50" s="89"/>
+      <c r="J50" s="89"/>
+      <c r="K50" s="89"/>
+      <c r="L50" s="89"/>
+      <c r="M50" s="89"/>
+      <c r="N50" s="89"/>
+      <c r="O50" s="89"/>
+      <c r="P50" s="89"/>
+      <c r="Q50" s="89"/>
+      <c r="R50" s="89"/>
+      <c r="S50" s="89"/>
+      <c r="T50" s="89"/>
+      <c r="U50" s="89"/>
+      <c r="V50" s="89"/>
       <c r="W50" s="79"/>
       <c r="X50" s="79"/>
       <c r="Y50" s="79"/>
@@ -83509,28 +83474,28 @@
       <c r="AM50" s="7"/>
     </row>
     <row r="51" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A51" s="87"/>
-      <c r="B51" s="87"/>
-      <c r="C51" s="87"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="87"/>
-      <c r="H51" s="87"/>
-      <c r="I51" s="87"/>
-      <c r="J51" s="87"/>
-      <c r="K51" s="87"/>
-      <c r="L51" s="87"/>
-      <c r="M51" s="87"/>
-      <c r="N51" s="87"/>
-      <c r="O51" s="87"/>
-      <c r="P51" s="87"/>
-      <c r="Q51" s="87"/>
-      <c r="R51" s="87"/>
-      <c r="S51" s="87"/>
-      <c r="T51" s="87"/>
-      <c r="U51" s="87"/>
-      <c r="V51" s="87"/>
+      <c r="A51" s="89"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="89"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="89"/>
+      <c r="J51" s="89"/>
+      <c r="K51" s="89"/>
+      <c r="L51" s="89"/>
+      <c r="M51" s="89"/>
+      <c r="N51" s="89"/>
+      <c r="O51" s="89"/>
+      <c r="P51" s="89"/>
+      <c r="Q51" s="89"/>
+      <c r="R51" s="89"/>
+      <c r="S51" s="89"/>
+      <c r="T51" s="89"/>
+      <c r="U51" s="89"/>
+      <c r="V51" s="89"/>
       <c r="W51" s="79"/>
       <c r="X51" s="79"/>
       <c r="Y51" s="79"/>
@@ -83550,30 +83515,30 @@
       <c r="AM51" s="7"/>
     </row>
     <row r="52" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A52" s="90" t="s">
+      <c r="A52" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="90"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="90"/>
-      <c r="H52" s="90"/>
-      <c r="I52" s="90"/>
-      <c r="J52" s="90"/>
-      <c r="K52" s="90"/>
-      <c r="L52" s="90"/>
-      <c r="M52" s="90"/>
-      <c r="N52" s="90"/>
-      <c r="O52" s="90"/>
-      <c r="P52" s="90"/>
-      <c r="Q52" s="90"/>
-      <c r="R52" s="90"/>
-      <c r="S52" s="90"/>
-      <c r="T52" s="90"/>
-      <c r="U52" s="90"/>
-      <c r="V52" s="90"/>
+      <c r="B52" s="83"/>
+      <c r="C52" s="83"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="83"/>
+      <c r="H52" s="83"/>
+      <c r="I52" s="83"/>
+      <c r="J52" s="83"/>
+      <c r="K52" s="83"/>
+      <c r="L52" s="83"/>
+      <c r="M52" s="83"/>
+      <c r="N52" s="83"/>
+      <c r="O52" s="83"/>
+      <c r="P52" s="83"/>
+      <c r="Q52" s="83"/>
+      <c r="R52" s="83"/>
+      <c r="S52" s="83"/>
+      <c r="T52" s="83"/>
+      <c r="U52" s="83"/>
+      <c r="V52" s="83"/>
       <c r="W52" s="79"/>
       <c r="X52" s="79"/>
       <c r="Y52" s="79"/>
@@ -83593,30 +83558,30 @@
       <c r="AM52" s="7"/>
     </row>
     <row r="53" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A53" s="85" t="s">
+      <c r="A53" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="85"/>
-      <c r="C53" s="85"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="85"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="85"/>
-      <c r="H53" s="85"/>
-      <c r="I53" s="85"/>
-      <c r="J53" s="85"/>
-      <c r="K53" s="85"/>
-      <c r="L53" s="85"/>
-      <c r="M53" s="85"/>
-      <c r="N53" s="85"/>
-      <c r="O53" s="85"/>
-      <c r="P53" s="85"/>
-      <c r="Q53" s="85"/>
-      <c r="R53" s="85"/>
-      <c r="S53" s="85"/>
-      <c r="T53" s="85"/>
-      <c r="U53" s="85"/>
-      <c r="V53" s="85"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="84"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="84"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="84"/>
+      <c r="N53" s="84"/>
+      <c r="O53" s="84"/>
+      <c r="P53" s="84"/>
+      <c r="Q53" s="84"/>
+      <c r="R53" s="84"/>
+      <c r="S53" s="84"/>
+      <c r="T53" s="84"/>
+      <c r="U53" s="84"/>
+      <c r="V53" s="84"/>
       <c r="W53" s="79"/>
       <c r="X53" s="79"/>
       <c r="Y53" s="79"/>
@@ -83636,58 +83601,58 @@
       <c r="AM53" s="7"/>
     </row>
     <row r="54" spans="1:39" s="14" customFormat="1" ht="38.85" customHeight="1">
-      <c r="A54" s="91" t="s">
+      <c r="A54" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="91"/>
-      <c r="C54" s="91"/>
-      <c r="D54" s="91"/>
-      <c r="E54" s="91"/>
-      <c r="F54" s="91"/>
-      <c r="G54" s="91"/>
-      <c r="H54" s="91"/>
-      <c r="I54" s="91"/>
-      <c r="J54" s="91"/>
-      <c r="K54" s="91"/>
-      <c r="L54" s="91"/>
-      <c r="M54" s="91"/>
-      <c r="N54" s="91"/>
-      <c r="O54" s="91"/>
-      <c r="P54" s="91"/>
-      <c r="Q54" s="91"/>
-      <c r="R54" s="91"/>
-      <c r="S54" s="91"/>
-      <c r="T54" s="91"/>
-      <c r="U54" s="91"/>
-      <c r="V54" s="91"/>
+      <c r="B54" s="85"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="85"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="85"/>
+      <c r="H54" s="85"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="85"/>
+      <c r="K54" s="85"/>
+      <c r="L54" s="85"/>
+      <c r="M54" s="85"/>
+      <c r="N54" s="85"/>
+      <c r="O54" s="85"/>
+      <c r="P54" s="85"/>
+      <c r="Q54" s="85"/>
+      <c r="R54" s="85"/>
+      <c r="S54" s="85"/>
+      <c r="T54" s="85"/>
+      <c r="U54" s="85"/>
+      <c r="V54" s="85"/>
       <c r="AL54" s="7"/>
       <c r="AM54" s="7"/>
     </row>
     <row r="55" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A55" s="85" t="s">
+      <c r="A55" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="85"/>
-      <c r="C55" s="85"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="85"/>
-      <c r="F55" s="85"/>
-      <c r="G55" s="85"/>
-      <c r="H55" s="85"/>
-      <c r="I55" s="85"/>
-      <c r="J55" s="85"/>
-      <c r="K55" s="85"/>
-      <c r="L55" s="85"/>
-      <c r="M55" s="85"/>
-      <c r="N55" s="85"/>
-      <c r="O55" s="85"/>
-      <c r="P55" s="85"/>
-      <c r="Q55" s="85"/>
-      <c r="R55" s="85"/>
-      <c r="S55" s="85"/>
-      <c r="T55" s="85"/>
-      <c r="U55" s="85"/>
-      <c r="V55" s="85"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="84"/>
+      <c r="G55" s="84"/>
+      <c r="H55" s="84"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="84"/>
+      <c r="K55" s="84"/>
+      <c r="L55" s="84"/>
+      <c r="M55" s="84"/>
+      <c r="N55" s="84"/>
+      <c r="O55" s="84"/>
+      <c r="P55" s="84"/>
+      <c r="Q55" s="84"/>
+      <c r="R55" s="84"/>
+      <c r="S55" s="84"/>
+      <c r="T55" s="84"/>
+      <c r="U55" s="84"/>
+      <c r="V55" s="84"/>
       <c r="W55" s="79"/>
       <c r="X55" s="79"/>
       <c r="Y55" s="79"/>
@@ -83707,30 +83672,30 @@
       <c r="AM55" s="7"/>
     </row>
     <row r="56" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A56" s="85" t="s">
+      <c r="A56" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="85"/>
-      <c r="C56" s="85"/>
-      <c r="D56" s="85"/>
-      <c r="E56" s="85"/>
-      <c r="F56" s="85"/>
-      <c r="G56" s="85"/>
-      <c r="H56" s="85"/>
-      <c r="I56" s="85"/>
-      <c r="J56" s="85"/>
-      <c r="K56" s="85"/>
-      <c r="L56" s="85"/>
-      <c r="M56" s="85"/>
-      <c r="N56" s="85"/>
-      <c r="O56" s="85"/>
-      <c r="P56" s="85"/>
-      <c r="Q56" s="85"/>
-      <c r="R56" s="85"/>
-      <c r="S56" s="85"/>
-      <c r="T56" s="85"/>
-      <c r="U56" s="85"/>
-      <c r="V56" s="85"/>
+      <c r="B56" s="84"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="84"/>
+      <c r="F56" s="84"/>
+      <c r="G56" s="84"/>
+      <c r="H56" s="84"/>
+      <c r="I56" s="84"/>
+      <c r="J56" s="84"/>
+      <c r="K56" s="84"/>
+      <c r="L56" s="84"/>
+      <c r="M56" s="84"/>
+      <c r="N56" s="84"/>
+      <c r="O56" s="84"/>
+      <c r="P56" s="84"/>
+      <c r="Q56" s="84"/>
+      <c r="R56" s="84"/>
+      <c r="S56" s="84"/>
+      <c r="T56" s="84"/>
+      <c r="U56" s="84"/>
+      <c r="V56" s="84"/>
       <c r="W56" s="79"/>
       <c r="X56" s="79"/>
       <c r="Y56" s="79"/>
@@ -83750,30 +83715,30 @@
       <c r="AM56" s="7"/>
     </row>
     <row r="57" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A57" s="83" t="s">
+      <c r="A57" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="83"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="83"/>
-      <c r="E57" s="83"/>
-      <c r="F57" s="83"/>
-      <c r="G57" s="83"/>
-      <c r="H57" s="83"/>
-      <c r="I57" s="83"/>
-      <c r="J57" s="83"/>
-      <c r="K57" s="83"/>
-      <c r="L57" s="83"/>
-      <c r="M57" s="83"/>
-      <c r="N57" s="83"/>
-      <c r="O57" s="83"/>
-      <c r="P57" s="83"/>
-      <c r="Q57" s="83"/>
-      <c r="R57" s="83"/>
-      <c r="S57" s="83"/>
-      <c r="T57" s="83"/>
-      <c r="U57" s="83"/>
-      <c r="V57" s="83"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="92"/>
+      <c r="E57" s="92"/>
+      <c r="F57" s="92"/>
+      <c r="G57" s="92"/>
+      <c r="H57" s="92"/>
+      <c r="I57" s="92"/>
+      <c r="J57" s="92"/>
+      <c r="K57" s="92"/>
+      <c r="L57" s="92"/>
+      <c r="M57" s="92"/>
+      <c r="N57" s="92"/>
+      <c r="O57" s="92"/>
+      <c r="P57" s="92"/>
+      <c r="Q57" s="92"/>
+      <c r="R57" s="92"/>
+      <c r="S57" s="92"/>
+      <c r="T57" s="92"/>
+      <c r="U57" s="92"/>
+      <c r="V57" s="92"/>
       <c r="W57" s="79"/>
       <c r="X57" s="79"/>
       <c r="Y57" s="79"/>
@@ -83793,28 +83758,28 @@
       <c r="AM57" s="7"/>
     </row>
     <row r="58" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A58" s="89"/>
-      <c r="B58" s="89"/>
-      <c r="C58" s="89"/>
-      <c r="D58" s="89"/>
-      <c r="E58" s="89"/>
-      <c r="F58" s="89"/>
-      <c r="G58" s="89"/>
-      <c r="H58" s="89"/>
-      <c r="I58" s="89"/>
-      <c r="J58" s="89"/>
-      <c r="K58" s="89"/>
-      <c r="L58" s="89"/>
-      <c r="M58" s="89"/>
-      <c r="N58" s="89"/>
-      <c r="O58" s="89"/>
-      <c r="P58" s="89"/>
-      <c r="Q58" s="89"/>
-      <c r="R58" s="89"/>
-      <c r="S58" s="89"/>
-      <c r="T58" s="89"/>
-      <c r="U58" s="89"/>
-      <c r="V58" s="89"/>
+      <c r="A58" s="93"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="93"/>
+      <c r="G58" s="93"/>
+      <c r="H58" s="93"/>
+      <c r="I58" s="93"/>
+      <c r="J58" s="93"/>
+      <c r="K58" s="93"/>
+      <c r="L58" s="93"/>
+      <c r="M58" s="93"/>
+      <c r="N58" s="93"/>
+      <c r="O58" s="93"/>
+      <c r="P58" s="93"/>
+      <c r="Q58" s="93"/>
+      <c r="R58" s="93"/>
+      <c r="S58" s="93"/>
+      <c r="T58" s="93"/>
+      <c r="U58" s="93"/>
+      <c r="V58" s="93"/>
       <c r="W58" s="79"/>
       <c r="X58" s="79"/>
       <c r="Y58" s="79"/>
@@ -83834,30 +83799,30 @@
       <c r="AM58" s="7"/>
     </row>
     <row r="59" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A59" s="88" t="s">
+      <c r="A59" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="88"/>
-      <c r="G59" s="88"/>
-      <c r="H59" s="88"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="88"/>
-      <c r="K59" s="88"/>
-      <c r="L59" s="88"/>
-      <c r="M59" s="88"/>
-      <c r="N59" s="88"/>
-      <c r="O59" s="88"/>
-      <c r="P59" s="88"/>
-      <c r="Q59" s="88"/>
-      <c r="R59" s="88"/>
-      <c r="S59" s="88"/>
-      <c r="T59" s="88"/>
-      <c r="U59" s="88"/>
-      <c r="V59" s="88"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="94"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
+      <c r="J59" s="94"/>
+      <c r="K59" s="94"/>
+      <c r="L59" s="94"/>
+      <c r="M59" s="94"/>
+      <c r="N59" s="94"/>
+      <c r="O59" s="94"/>
+      <c r="P59" s="94"/>
+      <c r="Q59" s="94"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="94"/>
+      <c r="T59" s="94"/>
+      <c r="U59" s="94"/>
+      <c r="V59" s="94"/>
       <c r="W59" s="79"/>
       <c r="X59" s="79"/>
       <c r="Y59" s="79"/>
@@ -83877,30 +83842,30 @@
       <c r="AM59" s="7"/>
     </row>
     <row r="60" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A60" s="88" t="s">
+      <c r="A60" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="88"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
-      <c r="E60" s="88"/>
-      <c r="F60" s="88"/>
-      <c r="G60" s="88"/>
-      <c r="H60" s="88"/>
-      <c r="I60" s="88"/>
-      <c r="J60" s="88"/>
-      <c r="K60" s="88"/>
-      <c r="L60" s="88"/>
-      <c r="M60" s="88"/>
-      <c r="N60" s="88"/>
-      <c r="O60" s="88"/>
-      <c r="P60" s="88"/>
-      <c r="Q60" s="88"/>
-      <c r="R60" s="88"/>
-      <c r="S60" s="88"/>
-      <c r="T60" s="88"/>
-      <c r="U60" s="88"/>
-      <c r="V60" s="88"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="94"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="94"/>
+      <c r="F60" s="94"/>
+      <c r="G60" s="94"/>
+      <c r="H60" s="94"/>
+      <c r="I60" s="94"/>
+      <c r="J60" s="94"/>
+      <c r="K60" s="94"/>
+      <c r="L60" s="94"/>
+      <c r="M60" s="94"/>
+      <c r="N60" s="94"/>
+      <c r="O60" s="94"/>
+      <c r="P60" s="94"/>
+      <c r="Q60" s="94"/>
+      <c r="R60" s="94"/>
+      <c r="S60" s="94"/>
+      <c r="T60" s="94"/>
+      <c r="U60" s="94"/>
+      <c r="V60" s="94"/>
       <c r="W60" s="79"/>
       <c r="X60" s="79"/>
       <c r="Y60" s="79"/>
@@ -83920,30 +83885,30 @@
       <c r="AM60" s="7"/>
     </row>
     <row r="61" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A61" s="82" t="s">
+      <c r="A61" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="B61" s="82"/>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="82"/>
-      <c r="F61" s="82"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="82"/>
-      <c r="J61" s="82"/>
-      <c r="K61" s="82"/>
-      <c r="L61" s="82"/>
-      <c r="M61" s="82"/>
-      <c r="N61" s="82"/>
-      <c r="O61" s="82"/>
-      <c r="P61" s="82"/>
-      <c r="Q61" s="82"/>
-      <c r="R61" s="82"/>
-      <c r="S61" s="82"/>
-      <c r="T61" s="82"/>
-      <c r="U61" s="82"/>
-      <c r="V61" s="82"/>
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
+      <c r="D61" s="95"/>
+      <c r="E61" s="95"/>
+      <c r="F61" s="95"/>
+      <c r="G61" s="95"/>
+      <c r="H61" s="95"/>
+      <c r="I61" s="95"/>
+      <c r="J61" s="95"/>
+      <c r="K61" s="95"/>
+      <c r="L61" s="95"/>
+      <c r="M61" s="95"/>
+      <c r="N61" s="95"/>
+      <c r="O61" s="95"/>
+      <c r="P61" s="95"/>
+      <c r="Q61" s="95"/>
+      <c r="R61" s="95"/>
+      <c r="S61" s="95"/>
+      <c r="T61" s="95"/>
+      <c r="U61" s="95"/>
+      <c r="V61" s="95"/>
       <c r="W61" s="79"/>
       <c r="X61" s="79"/>
       <c r="Y61" s="79"/>
@@ -83963,30 +83928,30 @@
       <c r="AM61" s="7"/>
     </row>
     <row r="62" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A62" s="86" t="s">
+      <c r="A62" s="96" t="s">
         <v>986</v>
       </c>
-      <c r="B62" s="86"/>
-      <c r="C62" s="86"/>
-      <c r="D62" s="86"/>
-      <c r="E62" s="86"/>
-      <c r="F62" s="86"/>
-      <c r="G62" s="86"/>
-      <c r="H62" s="86"/>
-      <c r="I62" s="86"/>
-      <c r="J62" s="86"/>
-      <c r="K62" s="86"/>
-      <c r="L62" s="86"/>
-      <c r="M62" s="86"/>
-      <c r="N62" s="86"/>
-      <c r="O62" s="86"/>
-      <c r="P62" s="86"/>
-      <c r="Q62" s="86"/>
-      <c r="R62" s="86"/>
-      <c r="S62" s="86"/>
-      <c r="T62" s="86"/>
-      <c r="U62" s="86"/>
-      <c r="V62" s="86"/>
+      <c r="B62" s="96"/>
+      <c r="C62" s="96"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="96"/>
+      <c r="F62" s="96"/>
+      <c r="G62" s="96"/>
+      <c r="H62" s="96"/>
+      <c r="I62" s="96"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
+      <c r="L62" s="96"/>
+      <c r="M62" s="96"/>
+      <c r="N62" s="96"/>
+      <c r="O62" s="96"/>
+      <c r="P62" s="96"/>
+      <c r="Q62" s="96"/>
+      <c r="R62" s="96"/>
+      <c r="S62" s="96"/>
+      <c r="T62" s="96"/>
+      <c r="U62" s="96"/>
+      <c r="V62" s="96"/>
       <c r="W62" s="79"/>
       <c r="X62" s="79"/>
       <c r="Y62" s="79"/>
@@ -84006,30 +83971,30 @@
       <c r="AM62" s="7"/>
     </row>
     <row r="63" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A63" s="84" t="s">
+      <c r="A63" s="97" t="s">
         <v>987</v>
       </c>
-      <c r="B63" s="84"/>
-      <c r="C63" s="84"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="84"/>
-      <c r="F63" s="84"/>
-      <c r="G63" s="84"/>
-      <c r="H63" s="84"/>
-      <c r="I63" s="84"/>
-      <c r="J63" s="84"/>
-      <c r="K63" s="84"/>
-      <c r="L63" s="84"/>
-      <c r="M63" s="84"/>
-      <c r="N63" s="84"/>
-      <c r="O63" s="84"/>
-      <c r="P63" s="84"/>
-      <c r="Q63" s="84"/>
-      <c r="R63" s="84"/>
-      <c r="S63" s="84"/>
-      <c r="T63" s="84"/>
-      <c r="U63" s="84"/>
-      <c r="V63" s="84"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="97"/>
+      <c r="G63" s="97"/>
+      <c r="H63" s="97"/>
+      <c r="I63" s="97"/>
+      <c r="J63" s="97"/>
+      <c r="K63" s="97"/>
+      <c r="L63" s="97"/>
+      <c r="M63" s="97"/>
+      <c r="N63" s="97"/>
+      <c r="O63" s="97"/>
+      <c r="P63" s="97"/>
+      <c r="Q63" s="97"/>
+      <c r="R63" s="97"/>
+      <c r="S63" s="97"/>
+      <c r="T63" s="97"/>
+      <c r="U63" s="97"/>
+      <c r="V63" s="97"/>
       <c r="W63" s="79"/>
       <c r="X63" s="79"/>
       <c r="Y63" s="79"/>
@@ -84049,30 +84014,30 @@
       <c r="AM63" s="7"/>
     </row>
     <row r="64" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A64" s="84" t="s">
+      <c r="A64" s="97" t="s">
         <v>988</v>
       </c>
-      <c r="B64" s="84"/>
-      <c r="C64" s="84"/>
-      <c r="D64" s="84"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="84"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="84"/>
-      <c r="I64" s="84"/>
-      <c r="J64" s="84"/>
-      <c r="K64" s="84"/>
-      <c r="L64" s="84"/>
-      <c r="M64" s="84"/>
-      <c r="N64" s="84"/>
-      <c r="O64" s="84"/>
-      <c r="P64" s="84"/>
-      <c r="Q64" s="84"/>
-      <c r="R64" s="84"/>
-      <c r="S64" s="84"/>
-      <c r="T64" s="84"/>
-      <c r="U64" s="84"/>
-      <c r="V64" s="84"/>
+      <c r="B64" s="97"/>
+      <c r="C64" s="97"/>
+      <c r="D64" s="97"/>
+      <c r="E64" s="97"/>
+      <c r="F64" s="97"/>
+      <c r="G64" s="97"/>
+      <c r="H64" s="97"/>
+      <c r="I64" s="97"/>
+      <c r="J64" s="97"/>
+      <c r="K64" s="97"/>
+      <c r="L64" s="97"/>
+      <c r="M64" s="97"/>
+      <c r="N64" s="97"/>
+      <c r="O64" s="97"/>
+      <c r="P64" s="97"/>
+      <c r="Q64" s="97"/>
+      <c r="R64" s="97"/>
+      <c r="S64" s="97"/>
+      <c r="T64" s="97"/>
+      <c r="U64" s="97"/>
+      <c r="V64" s="97"/>
       <c r="W64" s="79"/>
       <c r="X64" s="79"/>
       <c r="Y64" s="79"/>
@@ -84092,30 +84057,30 @@
       <c r="AM64" s="7"/>
     </row>
     <row r="65" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A65" s="84" t="s">
+      <c r="A65" s="97" t="s">
         <v>989</v>
       </c>
-      <c r="B65" s="84"/>
-      <c r="C65" s="84"/>
-      <c r="D65" s="84"/>
-      <c r="E65" s="84"/>
-      <c r="F65" s="84"/>
-      <c r="G65" s="84"/>
-      <c r="H65" s="84"/>
-      <c r="I65" s="84"/>
-      <c r="J65" s="84"/>
-      <c r="K65" s="84"/>
-      <c r="L65" s="84"/>
-      <c r="M65" s="84"/>
-      <c r="N65" s="84"/>
-      <c r="O65" s="84"/>
-      <c r="P65" s="84"/>
-      <c r="Q65" s="84"/>
-      <c r="R65" s="84"/>
-      <c r="S65" s="84"/>
-      <c r="T65" s="84"/>
-      <c r="U65" s="84"/>
-      <c r="V65" s="84"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="97"/>
+      <c r="D65" s="97"/>
+      <c r="E65" s="97"/>
+      <c r="F65" s="97"/>
+      <c r="G65" s="97"/>
+      <c r="H65" s="97"/>
+      <c r="I65" s="97"/>
+      <c r="J65" s="97"/>
+      <c r="K65" s="97"/>
+      <c r="L65" s="97"/>
+      <c r="M65" s="97"/>
+      <c r="N65" s="97"/>
+      <c r="O65" s="97"/>
+      <c r="P65" s="97"/>
+      <c r="Q65" s="97"/>
+      <c r="R65" s="97"/>
+      <c r="S65" s="97"/>
+      <c r="T65" s="97"/>
+      <c r="U65" s="97"/>
+      <c r="V65" s="97"/>
       <c r="W65" s="79"/>
       <c r="X65" s="79"/>
       <c r="Y65" s="79"/>
@@ -84135,30 +84100,30 @@
       <c r="AM65" s="7"/>
     </row>
     <row r="66" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A66" s="84" t="s">
+      <c r="A66" s="97" t="s">
         <v>1602</v>
       </c>
-      <c r="B66" s="84"/>
-      <c r="C66" s="84"/>
-      <c r="D66" s="84"/>
-      <c r="E66" s="84"/>
-      <c r="F66" s="84"/>
-      <c r="G66" s="84"/>
-      <c r="H66" s="84"/>
-      <c r="I66" s="84"/>
-      <c r="J66" s="84"/>
-      <c r="K66" s="84"/>
-      <c r="L66" s="84"/>
-      <c r="M66" s="84"/>
-      <c r="N66" s="84"/>
-      <c r="O66" s="84"/>
-      <c r="P66" s="84"/>
-      <c r="Q66" s="84"/>
-      <c r="R66" s="84"/>
-      <c r="S66" s="84"/>
-      <c r="T66" s="84"/>
-      <c r="U66" s="84"/>
-      <c r="V66" s="84"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="97"/>
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="H66" s="97"/>
+      <c r="I66" s="97"/>
+      <c r="J66" s="97"/>
+      <c r="K66" s="97"/>
+      <c r="L66" s="97"/>
+      <c r="M66" s="97"/>
+      <c r="N66" s="97"/>
+      <c r="O66" s="97"/>
+      <c r="P66" s="97"/>
+      <c r="Q66" s="97"/>
+      <c r="R66" s="97"/>
+      <c r="S66" s="97"/>
+      <c r="T66" s="97"/>
+      <c r="U66" s="97"/>
+      <c r="V66" s="97"/>
       <c r="W66" s="79"/>
       <c r="X66" s="79"/>
       <c r="Y66" s="79"/>
@@ -84178,30 +84143,30 @@
       <c r="AM66" s="7"/>
     </row>
     <row r="67" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A67" s="82" t="s">
+      <c r="A67" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="B67" s="82"/>
-      <c r="C67" s="82"/>
-      <c r="D67" s="82"/>
-      <c r="E67" s="82"/>
-      <c r="F67" s="82"/>
-      <c r="G67" s="82"/>
-      <c r="H67" s="82"/>
-      <c r="I67" s="82"/>
-      <c r="J67" s="82"/>
-      <c r="K67" s="82"/>
-      <c r="L67" s="82"/>
-      <c r="M67" s="82"/>
-      <c r="N67" s="82"/>
-      <c r="O67" s="82"/>
-      <c r="P67" s="82"/>
-      <c r="Q67" s="82"/>
-      <c r="R67" s="82"/>
-      <c r="S67" s="82"/>
-      <c r="T67" s="82"/>
-      <c r="U67" s="82"/>
-      <c r="V67" s="82"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="95"/>
+      <c r="D67" s="95"/>
+      <c r="E67" s="95"/>
+      <c r="F67" s="95"/>
+      <c r="G67" s="95"/>
+      <c r="H67" s="95"/>
+      <c r="I67" s="95"/>
+      <c r="J67" s="95"/>
+      <c r="K67" s="95"/>
+      <c r="L67" s="95"/>
+      <c r="M67" s="95"/>
+      <c r="N67" s="95"/>
+      <c r="O67" s="95"/>
+      <c r="P67" s="95"/>
+      <c r="Q67" s="95"/>
+      <c r="R67" s="95"/>
+      <c r="S67" s="95"/>
+      <c r="T67" s="95"/>
+      <c r="U67" s="95"/>
+      <c r="V67" s="95"/>
       <c r="W67" s="79"/>
       <c r="X67" s="79"/>
       <c r="Y67" s="79"/>
@@ -84221,30 +84186,30 @@
       <c r="AM67" s="7"/>
     </row>
     <row r="68" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A68" s="84" t="s">
+      <c r="A68" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="84"/>
-      <c r="C68" s="84"/>
-      <c r="D68" s="84"/>
-      <c r="E68" s="84"/>
-      <c r="F68" s="84"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="84"/>
-      <c r="I68" s="84"/>
-      <c r="J68" s="84"/>
-      <c r="K68" s="84"/>
-      <c r="L68" s="84"/>
-      <c r="M68" s="84"/>
-      <c r="N68" s="84"/>
-      <c r="O68" s="84"/>
-      <c r="P68" s="84"/>
-      <c r="Q68" s="84"/>
-      <c r="R68" s="84"/>
-      <c r="S68" s="84"/>
-      <c r="T68" s="84"/>
-      <c r="U68" s="84"/>
-      <c r="V68" s="84"/>
+      <c r="B68" s="97"/>
+      <c r="C68" s="97"/>
+      <c r="D68" s="97"/>
+      <c r="E68" s="97"/>
+      <c r="F68" s="97"/>
+      <c r="G68" s="97"/>
+      <c r="H68" s="97"/>
+      <c r="I68" s="97"/>
+      <c r="J68" s="97"/>
+      <c r="K68" s="97"/>
+      <c r="L68" s="97"/>
+      <c r="M68" s="97"/>
+      <c r="N68" s="97"/>
+      <c r="O68" s="97"/>
+      <c r="P68" s="97"/>
+      <c r="Q68" s="97"/>
+      <c r="R68" s="97"/>
+      <c r="S68" s="97"/>
+      <c r="T68" s="97"/>
+      <c r="U68" s="97"/>
+      <c r="V68" s="97"/>
       <c r="W68" s="79"/>
       <c r="X68" s="79"/>
       <c r="Y68" s="79"/>
@@ -84264,30 +84229,30 @@
       <c r="AM68" s="7"/>
     </row>
     <row r="69" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A69" s="84" t="s">
+      <c r="A69" s="97" t="s">
         <v>990</v>
       </c>
-      <c r="B69" s="84"/>
-      <c r="C69" s="84"/>
-      <c r="D69" s="84"/>
-      <c r="E69" s="84"/>
-      <c r="F69" s="84"/>
-      <c r="G69" s="84"/>
-      <c r="H69" s="84"/>
-      <c r="I69" s="84"/>
-      <c r="J69" s="84"/>
-      <c r="K69" s="84"/>
-      <c r="L69" s="84"/>
-      <c r="M69" s="84"/>
-      <c r="N69" s="84"/>
-      <c r="O69" s="84"/>
-      <c r="P69" s="84"/>
-      <c r="Q69" s="84"/>
-      <c r="R69" s="84"/>
-      <c r="S69" s="84"/>
-      <c r="T69" s="84"/>
-      <c r="U69" s="84"/>
-      <c r="V69" s="84"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="97"/>
+      <c r="D69" s="97"/>
+      <c r="E69" s="97"/>
+      <c r="F69" s="97"/>
+      <c r="G69" s="97"/>
+      <c r="H69" s="97"/>
+      <c r="I69" s="97"/>
+      <c r="J69" s="97"/>
+      <c r="K69" s="97"/>
+      <c r="L69" s="97"/>
+      <c r="M69" s="97"/>
+      <c r="N69" s="97"/>
+      <c r="O69" s="97"/>
+      <c r="P69" s="97"/>
+      <c r="Q69" s="97"/>
+      <c r="R69" s="97"/>
+      <c r="S69" s="97"/>
+      <c r="T69" s="97"/>
+      <c r="U69" s="97"/>
+      <c r="V69" s="97"/>
       <c r="W69" s="79"/>
       <c r="X69" s="79"/>
       <c r="Y69" s="79"/>
@@ -84307,30 +84272,30 @@
       <c r="AM69" s="7"/>
     </row>
     <row r="70" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A70" s="84" t="s">
+      <c r="A70" s="97" t="s">
         <v>991</v>
       </c>
-      <c r="B70" s="84"/>
-      <c r="C70" s="84"/>
-      <c r="D70" s="84"/>
-      <c r="E70" s="84"/>
-      <c r="F70" s="84"/>
-      <c r="G70" s="84"/>
-      <c r="H70" s="84"/>
-      <c r="I70" s="84"/>
-      <c r="J70" s="84"/>
-      <c r="K70" s="84"/>
-      <c r="L70" s="84"/>
-      <c r="M70" s="84"/>
-      <c r="N70" s="84"/>
-      <c r="O70" s="84"/>
-      <c r="P70" s="84"/>
-      <c r="Q70" s="84"/>
-      <c r="R70" s="84"/>
-      <c r="S70" s="84"/>
-      <c r="T70" s="84"/>
-      <c r="U70" s="84"/>
-      <c r="V70" s="84"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="97"/>
+      <c r="D70" s="97"/>
+      <c r="E70" s="97"/>
+      <c r="F70" s="97"/>
+      <c r="G70" s="97"/>
+      <c r="H70" s="97"/>
+      <c r="I70" s="97"/>
+      <c r="J70" s="97"/>
+      <c r="K70" s="97"/>
+      <c r="L70" s="97"/>
+      <c r="M70" s="97"/>
+      <c r="N70" s="97"/>
+      <c r="O70" s="97"/>
+      <c r="P70" s="97"/>
+      <c r="Q70" s="97"/>
+      <c r="R70" s="97"/>
+      <c r="S70" s="97"/>
+      <c r="T70" s="97"/>
+      <c r="U70" s="97"/>
+      <c r="V70" s="97"/>
       <c r="W70" s="79"/>
       <c r="X70" s="79"/>
       <c r="Y70" s="79"/>
@@ -84350,30 +84315,30 @@
       <c r="AM70" s="7"/>
     </row>
     <row r="71" spans="1:39" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="A71" s="84" t="s">
+      <c r="A71" s="97" t="s">
         <v>992</v>
       </c>
-      <c r="B71" s="84"/>
-      <c r="C71" s="84"/>
-      <c r="D71" s="84"/>
-      <c r="E71" s="84"/>
-      <c r="F71" s="84"/>
-      <c r="G71" s="84"/>
-      <c r="H71" s="84"/>
-      <c r="I71" s="84"/>
-      <c r="J71" s="84"/>
-      <c r="K71" s="84"/>
-      <c r="L71" s="84"/>
-      <c r="M71" s="84"/>
-      <c r="N71" s="84"/>
-      <c r="O71" s="84"/>
-      <c r="P71" s="84"/>
-      <c r="Q71" s="84"/>
-      <c r="R71" s="84"/>
-      <c r="S71" s="84"/>
-      <c r="T71" s="84"/>
-      <c r="U71" s="84"/>
-      <c r="V71" s="84"/>
+      <c r="B71" s="97"/>
+      <c r="C71" s="97"/>
+      <c r="D71" s="97"/>
+      <c r="E71" s="97"/>
+      <c r="F71" s="97"/>
+      <c r="G71" s="97"/>
+      <c r="H71" s="97"/>
+      <c r="I71" s="97"/>
+      <c r="J71" s="97"/>
+      <c r="K71" s="97"/>
+      <c r="L71" s="97"/>
+      <c r="M71" s="97"/>
+      <c r="N71" s="97"/>
+      <c r="O71" s="97"/>
+      <c r="P71" s="97"/>
+      <c r="Q71" s="97"/>
+      <c r="R71" s="97"/>
+      <c r="S71" s="97"/>
+      <c r="T71" s="97"/>
+      <c r="U71" s="97"/>
+      <c r="V71" s="97"/>
       <c r="W71" s="79"/>
       <c r="X71" s="79"/>
       <c r="Y71" s="79"/>
@@ -84393,30 +84358,30 @@
       <c r="AM71" s="7"/>
     </row>
     <row r="72" spans="1:39" s="14" customFormat="1" ht="12" customHeight="1">
-      <c r="A72" s="84" t="s">
+      <c r="A72" s="97" t="s">
         <v>1603</v>
       </c>
-      <c r="B72" s="84"/>
-      <c r="C72" s="84"/>
-      <c r="D72" s="84"/>
-      <c r="E72" s="84"/>
-      <c r="F72" s="84"/>
-      <c r="G72" s="84"/>
-      <c r="H72" s="84"/>
-      <c r="I72" s="84"/>
-      <c r="J72" s="84"/>
-      <c r="K72" s="84"/>
-      <c r="L72" s="84"/>
-      <c r="M72" s="84"/>
-      <c r="N72" s="84"/>
-      <c r="O72" s="84"/>
-      <c r="P72" s="84"/>
-      <c r="Q72" s="84"/>
-      <c r="R72" s="84"/>
-      <c r="S72" s="84"/>
-      <c r="T72" s="84"/>
-      <c r="U72" s="84"/>
-      <c r="V72" s="84"/>
+      <c r="B72" s="97"/>
+      <c r="C72" s="97"/>
+      <c r="D72" s="97"/>
+      <c r="E72" s="97"/>
+      <c r="F72" s="97"/>
+      <c r="G72" s="97"/>
+      <c r="H72" s="97"/>
+      <c r="I72" s="97"/>
+      <c r="J72" s="97"/>
+      <c r="K72" s="97"/>
+      <c r="L72" s="97"/>
+      <c r="M72" s="97"/>
+      <c r="N72" s="97"/>
+      <c r="O72" s="97"/>
+      <c r="P72" s="97"/>
+      <c r="Q72" s="97"/>
+      <c r="R72" s="97"/>
+      <c r="S72" s="97"/>
+      <c r="T72" s="97"/>
+      <c r="U72" s="97"/>
+      <c r="V72" s="97"/>
       <c r="W72" s="79"/>
       <c r="X72" s="79"/>
       <c r="Y72" s="79"/>
@@ -84436,30 +84401,30 @@
       <c r="AM72" s="7"/>
     </row>
     <row r="73" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A73" s="84" t="s">
+      <c r="A73" s="97" t="s">
         <v>1604</v>
       </c>
-      <c r="B73" s="84"/>
-      <c r="C73" s="84"/>
-      <c r="D73" s="84"/>
-      <c r="E73" s="84"/>
-      <c r="F73" s="84"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="84"/>
-      <c r="I73" s="84"/>
-      <c r="J73" s="84"/>
-      <c r="K73" s="84"/>
-      <c r="L73" s="84"/>
-      <c r="M73" s="84"/>
-      <c r="N73" s="84"/>
-      <c r="O73" s="84"/>
-      <c r="P73" s="84"/>
-      <c r="Q73" s="84"/>
-      <c r="R73" s="84"/>
-      <c r="S73" s="84"/>
-      <c r="T73" s="84"/>
-      <c r="U73" s="84"/>
-      <c r="V73" s="84"/>
+      <c r="B73" s="97"/>
+      <c r="C73" s="97"/>
+      <c r="D73" s="97"/>
+      <c r="E73" s="97"/>
+      <c r="F73" s="97"/>
+      <c r="G73" s="97"/>
+      <c r="H73" s="97"/>
+      <c r="I73" s="97"/>
+      <c r="J73" s="97"/>
+      <c r="K73" s="97"/>
+      <c r="L73" s="97"/>
+      <c r="M73" s="97"/>
+      <c r="N73" s="97"/>
+      <c r="O73" s="97"/>
+      <c r="P73" s="97"/>
+      <c r="Q73" s="97"/>
+      <c r="R73" s="97"/>
+      <c r="S73" s="97"/>
+      <c r="T73" s="97"/>
+      <c r="U73" s="97"/>
+      <c r="V73" s="97"/>
       <c r="W73" s="79"/>
       <c r="X73" s="79"/>
       <c r="Y73" s="79"/>
@@ -84479,30 +84444,30 @@
       <c r="AM73" s="7"/>
     </row>
     <row r="74" spans="1:39" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A74" s="81" t="s">
+      <c r="A74" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B74" s="81"/>
-      <c r="C74" s="81"/>
-      <c r="D74" s="81"/>
-      <c r="E74" s="81"/>
-      <c r="F74" s="81"/>
-      <c r="G74" s="81"/>
-      <c r="H74" s="81"/>
-      <c r="I74" s="81"/>
-      <c r="J74" s="81"/>
-      <c r="K74" s="81"/>
-      <c r="L74" s="81"/>
-      <c r="M74" s="81"/>
-      <c r="N74" s="81"/>
-      <c r="O74" s="81"/>
-      <c r="P74" s="81"/>
-      <c r="Q74" s="81"/>
-      <c r="R74" s="81"/>
-      <c r="S74" s="81"/>
-      <c r="T74" s="81"/>
-      <c r="U74" s="81"/>
-      <c r="V74" s="81"/>
+      <c r="B74" s="98"/>
+      <c r="C74" s="98"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="98"/>
+      <c r="F74" s="98"/>
+      <c r="G74" s="98"/>
+      <c r="H74" s="98"/>
+      <c r="I74" s="98"/>
+      <c r="J74" s="98"/>
+      <c r="K74" s="98"/>
+      <c r="L74" s="98"/>
+      <c r="M74" s="98"/>
+      <c r="N74" s="98"/>
+      <c r="O74" s="98"/>
+      <c r="P74" s="98"/>
+      <c r="Q74" s="98"/>
+      <c r="R74" s="98"/>
+      <c r="S74" s="98"/>
+      <c r="T74" s="98"/>
+      <c r="U74" s="98"/>
+      <c r="V74" s="98"/>
       <c r="W74" s="79"/>
       <c r="X74" s="79"/>
       <c r="Y74" s="79"/>
@@ -84522,30 +84487,30 @@
       <c r="AM74" s="7"/>
     </row>
     <row r="75" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A75" s="85" t="s">
+      <c r="A75" s="84" t="s">
         <v>993</v>
       </c>
-      <c r="B75" s="85"/>
-      <c r="C75" s="85"/>
-      <c r="D75" s="85"/>
-      <c r="E75" s="85"/>
-      <c r="F75" s="85"/>
-      <c r="G75" s="85"/>
-      <c r="H75" s="85"/>
-      <c r="I75" s="85"/>
-      <c r="J75" s="85"/>
-      <c r="K75" s="85"/>
-      <c r="L75" s="85"/>
-      <c r="M75" s="85"/>
-      <c r="N75" s="85"/>
-      <c r="O75" s="85"/>
-      <c r="P75" s="85"/>
-      <c r="Q75" s="85"/>
-      <c r="R75" s="85"/>
-      <c r="S75" s="85"/>
-      <c r="T75" s="85"/>
-      <c r="U75" s="85"/>
-      <c r="V75" s="85"/>
+      <c r="B75" s="84"/>
+      <c r="C75" s="84"/>
+      <c r="D75" s="84"/>
+      <c r="E75" s="84"/>
+      <c r="F75" s="84"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="84"/>
+      <c r="I75" s="84"/>
+      <c r="J75" s="84"/>
+      <c r="K75" s="84"/>
+      <c r="L75" s="84"/>
+      <c r="M75" s="84"/>
+      <c r="N75" s="84"/>
+      <c r="O75" s="84"/>
+      <c r="P75" s="84"/>
+      <c r="Q75" s="84"/>
+      <c r="R75" s="84"/>
+      <c r="S75" s="84"/>
+      <c r="T75" s="84"/>
+      <c r="U75" s="84"/>
+      <c r="V75" s="84"/>
       <c r="W75" s="79"/>
       <c r="X75" s="79"/>
       <c r="Y75" s="79"/>
@@ -84565,30 +84530,30 @@
       <c r="AM75" s="7"/>
     </row>
     <row r="76" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A76" s="84" t="s">
+      <c r="A76" s="97" t="s">
         <v>1605</v>
       </c>
-      <c r="B76" s="84"/>
-      <c r="C76" s="84"/>
-      <c r="D76" s="84"/>
-      <c r="E76" s="84"/>
-      <c r="F76" s="84"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="84"/>
-      <c r="I76" s="84"/>
-      <c r="J76" s="84"/>
-      <c r="K76" s="84"/>
-      <c r="L76" s="84"/>
-      <c r="M76" s="84"/>
-      <c r="N76" s="84"/>
-      <c r="O76" s="84"/>
-      <c r="P76" s="84"/>
-      <c r="Q76" s="84"/>
-      <c r="R76" s="84"/>
-      <c r="S76" s="84"/>
-      <c r="T76" s="84"/>
-      <c r="U76" s="84"/>
-      <c r="V76" s="84"/>
+      <c r="B76" s="97"/>
+      <c r="C76" s="97"/>
+      <c r="D76" s="97"/>
+      <c r="E76" s="97"/>
+      <c r="F76" s="97"/>
+      <c r="G76" s="97"/>
+      <c r="H76" s="97"/>
+      <c r="I76" s="97"/>
+      <c r="J76" s="97"/>
+      <c r="K76" s="97"/>
+      <c r="L76" s="97"/>
+      <c r="M76" s="97"/>
+      <c r="N76" s="97"/>
+      <c r="O76" s="97"/>
+      <c r="P76" s="97"/>
+      <c r="Q76" s="97"/>
+      <c r="R76" s="97"/>
+      <c r="S76" s="97"/>
+      <c r="T76" s="97"/>
+      <c r="U76" s="97"/>
+      <c r="V76" s="97"/>
       <c r="W76" s="79"/>
       <c r="X76" s="79"/>
       <c r="Y76" s="79"/>
@@ -84608,30 +84573,30 @@
       <c r="AM76" s="7"/>
     </row>
     <row r="77" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A77" s="81" t="s">
+      <c r="A77" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B77" s="81"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="81"/>
-      <c r="E77" s="81"/>
-      <c r="F77" s="81"/>
-      <c r="G77" s="81"/>
-      <c r="H77" s="81"/>
-      <c r="I77" s="81"/>
-      <c r="J77" s="81"/>
-      <c r="K77" s="81"/>
-      <c r="L77" s="81"/>
-      <c r="M77" s="81"/>
-      <c r="N77" s="81"/>
-      <c r="O77" s="81"/>
-      <c r="P77" s="81"/>
-      <c r="Q77" s="81"/>
-      <c r="R77" s="81"/>
-      <c r="S77" s="81"/>
-      <c r="T77" s="81"/>
-      <c r="U77" s="81"/>
-      <c r="V77" s="81"/>
+      <c r="B77" s="98"/>
+      <c r="C77" s="98"/>
+      <c r="D77" s="98"/>
+      <c r="E77" s="98"/>
+      <c r="F77" s="98"/>
+      <c r="G77" s="98"/>
+      <c r="H77" s="98"/>
+      <c r="I77" s="98"/>
+      <c r="J77" s="98"/>
+      <c r="K77" s="98"/>
+      <c r="L77" s="98"/>
+      <c r="M77" s="98"/>
+      <c r="N77" s="98"/>
+      <c r="O77" s="98"/>
+      <c r="P77" s="98"/>
+      <c r="Q77" s="98"/>
+      <c r="R77" s="98"/>
+      <c r="S77" s="98"/>
+      <c r="T77" s="98"/>
+      <c r="U77" s="98"/>
+      <c r="V77" s="98"/>
       <c r="W77" s="79"/>
       <c r="X77" s="79"/>
       <c r="Y77" s="79"/>
@@ -84651,30 +84616,30 @@
       <c r="AM77" s="7"/>
     </row>
     <row r="78" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A78" s="84" t="s">
+      <c r="A78" s="97" t="s">
         <v>994</v>
       </c>
-      <c r="B78" s="84"/>
-      <c r="C78" s="84"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="84"/>
-      <c r="F78" s="84"/>
-      <c r="G78" s="84"/>
-      <c r="H78" s="84"/>
-      <c r="I78" s="84"/>
-      <c r="J78" s="84"/>
-      <c r="K78" s="84"/>
-      <c r="L78" s="84"/>
-      <c r="M78" s="84"/>
-      <c r="N78" s="84"/>
-      <c r="O78" s="84"/>
-      <c r="P78" s="84"/>
-      <c r="Q78" s="84"/>
-      <c r="R78" s="84"/>
-      <c r="S78" s="84"/>
-      <c r="T78" s="84"/>
-      <c r="U78" s="84"/>
-      <c r="V78" s="84"/>
+      <c r="B78" s="97"/>
+      <c r="C78" s="97"/>
+      <c r="D78" s="97"/>
+      <c r="E78" s="97"/>
+      <c r="F78" s="97"/>
+      <c r="G78" s="97"/>
+      <c r="H78" s="97"/>
+      <c r="I78" s="97"/>
+      <c r="J78" s="97"/>
+      <c r="K78" s="97"/>
+      <c r="L78" s="97"/>
+      <c r="M78" s="97"/>
+      <c r="N78" s="97"/>
+      <c r="O78" s="97"/>
+      <c r="P78" s="97"/>
+      <c r="Q78" s="97"/>
+      <c r="R78" s="97"/>
+      <c r="S78" s="97"/>
+      <c r="T78" s="97"/>
+      <c r="U78" s="97"/>
+      <c r="V78" s="97"/>
       <c r="W78" s="79"/>
       <c r="X78" s="79"/>
       <c r="Y78" s="79"/>
@@ -84694,30 +84659,30 @@
       <c r="AM78" s="7"/>
     </row>
     <row r="79" spans="1:39" s="14" customFormat="1" ht="12" customHeight="1">
-      <c r="A79" s="84" t="s">
+      <c r="A79" s="97" t="s">
         <v>995</v>
       </c>
-      <c r="B79" s="84"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="84"/>
-      <c r="E79" s="84"/>
-      <c r="F79" s="84"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="84"/>
-      <c r="I79" s="84"/>
-      <c r="J79" s="84"/>
-      <c r="K79" s="84"/>
-      <c r="L79" s="84"/>
-      <c r="M79" s="84"/>
-      <c r="N79" s="84"/>
-      <c r="O79" s="84"/>
-      <c r="P79" s="84"/>
-      <c r="Q79" s="84"/>
-      <c r="R79" s="84"/>
-      <c r="S79" s="84"/>
-      <c r="T79" s="84"/>
-      <c r="U79" s="84"/>
-      <c r="V79" s="84"/>
+      <c r="B79" s="97"/>
+      <c r="C79" s="97"/>
+      <c r="D79" s="97"/>
+      <c r="E79" s="97"/>
+      <c r="F79" s="97"/>
+      <c r="G79" s="97"/>
+      <c r="H79" s="97"/>
+      <c r="I79" s="97"/>
+      <c r="J79" s="97"/>
+      <c r="K79" s="97"/>
+      <c r="L79" s="97"/>
+      <c r="M79" s="97"/>
+      <c r="N79" s="97"/>
+      <c r="O79" s="97"/>
+      <c r="P79" s="97"/>
+      <c r="Q79" s="97"/>
+      <c r="R79" s="97"/>
+      <c r="S79" s="97"/>
+      <c r="T79" s="97"/>
+      <c r="U79" s="97"/>
+      <c r="V79" s="97"/>
       <c r="W79" s="79"/>
       <c r="X79" s="79"/>
       <c r="Y79" s="79"/>
@@ -84737,30 +84702,30 @@
       <c r="AM79" s="7"/>
     </row>
     <row r="80" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A80" s="84" t="s">
+      <c r="A80" s="97" t="s">
         <v>1606</v>
       </c>
-      <c r="B80" s="84"/>
-      <c r="C80" s="84"/>
-      <c r="D80" s="84"/>
-      <c r="E80" s="84"/>
-      <c r="F80" s="84"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="84"/>
-      <c r="I80" s="84"/>
-      <c r="J80" s="84"/>
-      <c r="K80" s="84"/>
-      <c r="L80" s="84"/>
-      <c r="M80" s="84"/>
-      <c r="N80" s="84"/>
-      <c r="O80" s="84"/>
-      <c r="P80" s="84"/>
-      <c r="Q80" s="84"/>
-      <c r="R80" s="84"/>
-      <c r="S80" s="84"/>
-      <c r="T80" s="84"/>
-      <c r="U80" s="84"/>
-      <c r="V80" s="84"/>
+      <c r="B80" s="97"/>
+      <c r="C80" s="97"/>
+      <c r="D80" s="97"/>
+      <c r="E80" s="97"/>
+      <c r="F80" s="97"/>
+      <c r="G80" s="97"/>
+      <c r="H80" s="97"/>
+      <c r="I80" s="97"/>
+      <c r="J80" s="97"/>
+      <c r="K80" s="97"/>
+      <c r="L80" s="97"/>
+      <c r="M80" s="97"/>
+      <c r="N80" s="97"/>
+      <c r="O80" s="97"/>
+      <c r="P80" s="97"/>
+      <c r="Q80" s="97"/>
+      <c r="R80" s="97"/>
+      <c r="S80" s="97"/>
+      <c r="T80" s="97"/>
+      <c r="U80" s="97"/>
+      <c r="V80" s="97"/>
       <c r="W80" s="79"/>
       <c r="X80" s="79"/>
       <c r="Y80" s="79"/>
@@ -84780,30 +84745,30 @@
       <c r="AM80" s="7"/>
     </row>
     <row r="81" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A81" s="81" t="s">
+      <c r="A81" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="81"/>
-      <c r="C81" s="81"/>
-      <c r="D81" s="81"/>
-      <c r="E81" s="81"/>
-      <c r="F81" s="81"/>
-      <c r="G81" s="81"/>
-      <c r="H81" s="81"/>
-      <c r="I81" s="81"/>
-      <c r="J81" s="81"/>
-      <c r="K81" s="81"/>
-      <c r="L81" s="81"/>
-      <c r="M81" s="81"/>
-      <c r="N81" s="81"/>
-      <c r="O81" s="81"/>
-      <c r="P81" s="81"/>
-      <c r="Q81" s="81"/>
-      <c r="R81" s="81"/>
-      <c r="S81" s="81"/>
-      <c r="T81" s="81"/>
-      <c r="U81" s="81"/>
-      <c r="V81" s="81"/>
+      <c r="B81" s="98"/>
+      <c r="C81" s="98"/>
+      <c r="D81" s="98"/>
+      <c r="E81" s="98"/>
+      <c r="F81" s="98"/>
+      <c r="G81" s="98"/>
+      <c r="H81" s="98"/>
+      <c r="I81" s="98"/>
+      <c r="J81" s="98"/>
+      <c r="K81" s="98"/>
+      <c r="L81" s="98"/>
+      <c r="M81" s="98"/>
+      <c r="N81" s="98"/>
+      <c r="O81" s="98"/>
+      <c r="P81" s="98"/>
+      <c r="Q81" s="98"/>
+      <c r="R81" s="98"/>
+      <c r="S81" s="98"/>
+      <c r="T81" s="98"/>
+      <c r="U81" s="98"/>
+      <c r="V81" s="98"/>
       <c r="W81" s="79"/>
       <c r="X81" s="79"/>
       <c r="Y81" s="79"/>
@@ -84823,30 +84788,30 @@
       <c r="AM81" s="7"/>
     </row>
     <row r="82" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A82" s="84" t="s">
+      <c r="A82" s="97" t="s">
         <v>1607</v>
       </c>
-      <c r="B82" s="84"/>
-      <c r="C82" s="84"/>
-      <c r="D82" s="84"/>
-      <c r="E82" s="84"/>
-      <c r="F82" s="84"/>
-      <c r="G82" s="84"/>
-      <c r="H82" s="84"/>
-      <c r="I82" s="84"/>
-      <c r="J82" s="84"/>
-      <c r="K82" s="84"/>
-      <c r="L82" s="84"/>
-      <c r="M82" s="84"/>
-      <c r="N82" s="84"/>
-      <c r="O82" s="84"/>
-      <c r="P82" s="84"/>
-      <c r="Q82" s="84"/>
-      <c r="R82" s="84"/>
-      <c r="S82" s="84"/>
-      <c r="T82" s="84"/>
-      <c r="U82" s="84"/>
-      <c r="V82" s="84"/>
+      <c r="B82" s="97"/>
+      <c r="C82" s="97"/>
+      <c r="D82" s="97"/>
+      <c r="E82" s="97"/>
+      <c r="F82" s="97"/>
+      <c r="G82" s="97"/>
+      <c r="H82" s="97"/>
+      <c r="I82" s="97"/>
+      <c r="J82" s="97"/>
+      <c r="K82" s="97"/>
+      <c r="L82" s="97"/>
+      <c r="M82" s="97"/>
+      <c r="N82" s="97"/>
+      <c r="O82" s="97"/>
+      <c r="P82" s="97"/>
+      <c r="Q82" s="97"/>
+      <c r="R82" s="97"/>
+      <c r="S82" s="97"/>
+      <c r="T82" s="97"/>
+      <c r="U82" s="97"/>
+      <c r="V82" s="97"/>
       <c r="W82" s="79"/>
       <c r="X82" s="79"/>
       <c r="Y82" s="79"/>
@@ -84866,30 +84831,30 @@
       <c r="AM82" s="7"/>
     </row>
     <row r="83" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A83" s="81" t="s">
+      <c r="A83" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B83" s="81"/>
-      <c r="C83" s="81"/>
-      <c r="D83" s="81"/>
-      <c r="E83" s="81"/>
-      <c r="F83" s="81"/>
-      <c r="G83" s="81"/>
-      <c r="H83" s="81"/>
-      <c r="I83" s="81"/>
-      <c r="J83" s="81"/>
-      <c r="K83" s="81"/>
-      <c r="L83" s="81"/>
-      <c r="M83" s="81"/>
-      <c r="N83" s="81"/>
-      <c r="O83" s="81"/>
-      <c r="P83" s="81"/>
-      <c r="Q83" s="81"/>
-      <c r="R83" s="81"/>
-      <c r="S83" s="81"/>
-      <c r="T83" s="81"/>
-      <c r="U83" s="81"/>
-      <c r="V83" s="81"/>
+      <c r="B83" s="98"/>
+      <c r="C83" s="98"/>
+      <c r="D83" s="98"/>
+      <c r="E83" s="98"/>
+      <c r="F83" s="98"/>
+      <c r="G83" s="98"/>
+      <c r="H83" s="98"/>
+      <c r="I83" s="98"/>
+      <c r="J83" s="98"/>
+      <c r="K83" s="98"/>
+      <c r="L83" s="98"/>
+      <c r="M83" s="98"/>
+      <c r="N83" s="98"/>
+      <c r="O83" s="98"/>
+      <c r="P83" s="98"/>
+      <c r="Q83" s="98"/>
+      <c r="R83" s="98"/>
+      <c r="S83" s="98"/>
+      <c r="T83" s="98"/>
+      <c r="U83" s="98"/>
+      <c r="V83" s="98"/>
       <c r="W83" s="79"/>
       <c r="X83" s="79"/>
       <c r="Y83" s="79"/>
@@ -84909,30 +84874,30 @@
       <c r="AM83" s="7"/>
     </row>
     <row r="84" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A84" s="84" t="s">
+      <c r="A84" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="B84" s="84"/>
-      <c r="C84" s="84"/>
-      <c r="D84" s="84"/>
-      <c r="E84" s="84"/>
-      <c r="F84" s="84"/>
-      <c r="G84" s="84"/>
-      <c r="H84" s="84"/>
-      <c r="I84" s="84"/>
-      <c r="J84" s="84"/>
-      <c r="K84" s="84"/>
-      <c r="L84" s="84"/>
-      <c r="M84" s="84"/>
-      <c r="N84" s="84"/>
-      <c r="O84" s="84"/>
-      <c r="P84" s="84"/>
-      <c r="Q84" s="84"/>
-      <c r="R84" s="84"/>
-      <c r="S84" s="84"/>
-      <c r="T84" s="84"/>
-      <c r="U84" s="84"/>
-      <c r="V84" s="84"/>
+      <c r="B84" s="97"/>
+      <c r="C84" s="97"/>
+      <c r="D84" s="97"/>
+      <c r="E84" s="97"/>
+      <c r="F84" s="97"/>
+      <c r="G84" s="97"/>
+      <c r="H84" s="97"/>
+      <c r="I84" s="97"/>
+      <c r="J84" s="97"/>
+      <c r="K84" s="97"/>
+      <c r="L84" s="97"/>
+      <c r="M84" s="97"/>
+      <c r="N84" s="97"/>
+      <c r="O84" s="97"/>
+      <c r="P84" s="97"/>
+      <c r="Q84" s="97"/>
+      <c r="R84" s="97"/>
+      <c r="S84" s="97"/>
+      <c r="T84" s="97"/>
+      <c r="U84" s="97"/>
+      <c r="V84" s="97"/>
       <c r="W84" s="79"/>
       <c r="X84" s="79"/>
       <c r="Y84" s="79"/>
@@ -84952,30 +84917,30 @@
       <c r="AM84" s="7"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A85" s="84" t="s">
+      <c r="A85" s="97" t="s">
         <v>996</v>
       </c>
-      <c r="B85" s="84"/>
-      <c r="C85" s="84"/>
-      <c r="D85" s="84"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="84"/>
-      <c r="H85" s="84"/>
-      <c r="I85" s="84"/>
-      <c r="J85" s="84"/>
-      <c r="K85" s="84"/>
-      <c r="L85" s="84"/>
-      <c r="M85" s="84"/>
-      <c r="N85" s="84"/>
-      <c r="O85" s="84"/>
-      <c r="P85" s="84"/>
-      <c r="Q85" s="84"/>
-      <c r="R85" s="84"/>
-      <c r="S85" s="84"/>
-      <c r="T85" s="84"/>
-      <c r="U85" s="84"/>
-      <c r="V85" s="84"/>
+      <c r="B85" s="97"/>
+      <c r="C85" s="97"/>
+      <c r="D85" s="97"/>
+      <c r="E85" s="97"/>
+      <c r="F85" s="97"/>
+      <c r="G85" s="97"/>
+      <c r="H85" s="97"/>
+      <c r="I85" s="97"/>
+      <c r="J85" s="97"/>
+      <c r="K85" s="97"/>
+      <c r="L85" s="97"/>
+      <c r="M85" s="97"/>
+      <c r="N85" s="97"/>
+      <c r="O85" s="97"/>
+      <c r="P85" s="97"/>
+      <c r="Q85" s="97"/>
+      <c r="R85" s="97"/>
+      <c r="S85" s="97"/>
+      <c r="T85" s="97"/>
+      <c r="U85" s="97"/>
+      <c r="V85" s="97"/>
       <c r="W85" s="79"/>
       <c r="X85" s="79"/>
       <c r="Y85" s="79"/>
@@ -84995,30 +84960,30 @@
       <c r="AM85" s="7"/>
     </row>
     <row r="86" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A86" s="84" t="s">
+      <c r="A86" s="97" t="s">
         <v>1608</v>
       </c>
-      <c r="B86" s="84"/>
-      <c r="C86" s="84"/>
-      <c r="D86" s="84"/>
-      <c r="E86" s="84"/>
-      <c r="F86" s="84"/>
-      <c r="G86" s="84"/>
-      <c r="H86" s="84"/>
-      <c r="I86" s="84"/>
-      <c r="J86" s="84"/>
-      <c r="K86" s="84"/>
-      <c r="L86" s="84"/>
-      <c r="M86" s="84"/>
-      <c r="N86" s="84"/>
-      <c r="O86" s="84"/>
-      <c r="P86" s="84"/>
-      <c r="Q86" s="84"/>
-      <c r="R86" s="84"/>
-      <c r="S86" s="84"/>
-      <c r="T86" s="84"/>
-      <c r="U86" s="84"/>
-      <c r="V86" s="84"/>
+      <c r="B86" s="97"/>
+      <c r="C86" s="97"/>
+      <c r="D86" s="97"/>
+      <c r="E86" s="97"/>
+      <c r="F86" s="97"/>
+      <c r="G86" s="97"/>
+      <c r="H86" s="97"/>
+      <c r="I86" s="97"/>
+      <c r="J86" s="97"/>
+      <c r="K86" s="97"/>
+      <c r="L86" s="97"/>
+      <c r="M86" s="97"/>
+      <c r="N86" s="97"/>
+      <c r="O86" s="97"/>
+      <c r="P86" s="97"/>
+      <c r="Q86" s="97"/>
+      <c r="R86" s="97"/>
+      <c r="S86" s="97"/>
+      <c r="T86" s="97"/>
+      <c r="U86" s="97"/>
+      <c r="V86" s="97"/>
       <c r="W86" s="79"/>
       <c r="X86" s="79"/>
       <c r="Y86" s="79"/>
@@ -85038,30 +85003,30 @@
       <c r="AM86" s="7"/>
     </row>
     <row r="87" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A87" s="81" t="s">
+      <c r="A87" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B87" s="81"/>
-      <c r="C87" s="81"/>
-      <c r="D87" s="81"/>
-      <c r="E87" s="81"/>
-      <c r="F87" s="81"/>
-      <c r="G87" s="81"/>
-      <c r="H87" s="81"/>
-      <c r="I87" s="81"/>
-      <c r="J87" s="81"/>
-      <c r="K87" s="81"/>
-      <c r="L87" s="81"/>
-      <c r="M87" s="81"/>
-      <c r="N87" s="81"/>
-      <c r="O87" s="81"/>
-      <c r="P87" s="81"/>
-      <c r="Q87" s="81"/>
-      <c r="R87" s="81"/>
-      <c r="S87" s="81"/>
-      <c r="T87" s="81"/>
-      <c r="U87" s="81"/>
-      <c r="V87" s="81"/>
+      <c r="B87" s="98"/>
+      <c r="C87" s="98"/>
+      <c r="D87" s="98"/>
+      <c r="E87" s="98"/>
+      <c r="F87" s="98"/>
+      <c r="G87" s="98"/>
+      <c r="H87" s="98"/>
+      <c r="I87" s="98"/>
+      <c r="J87" s="98"/>
+      <c r="K87" s="98"/>
+      <c r="L87" s="98"/>
+      <c r="M87" s="98"/>
+      <c r="N87" s="98"/>
+      <c r="O87" s="98"/>
+      <c r="P87" s="98"/>
+      <c r="Q87" s="98"/>
+      <c r="R87" s="98"/>
+      <c r="S87" s="98"/>
+      <c r="T87" s="98"/>
+      <c r="U87" s="98"/>
+      <c r="V87" s="98"/>
       <c r="W87" s="79"/>
       <c r="X87" s="79"/>
       <c r="Y87" s="79"/>
@@ -85081,30 +85046,30 @@
       <c r="AM87" s="7"/>
     </row>
     <row r="88" spans="1:39" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A88" s="82" t="s">
+      <c r="A88" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="82"/>
-      <c r="C88" s="82"/>
-      <c r="D88" s="82"/>
-      <c r="E88" s="82"/>
-      <c r="F88" s="82"/>
-      <c r="G88" s="82"/>
-      <c r="H88" s="82"/>
-      <c r="I88" s="82"/>
-      <c r="J88" s="82"/>
-      <c r="K88" s="82"/>
-      <c r="L88" s="82"/>
-      <c r="M88" s="82"/>
-      <c r="N88" s="82"/>
-      <c r="O88" s="82"/>
-      <c r="P88" s="82"/>
-      <c r="Q88" s="82"/>
-      <c r="R88" s="82"/>
-      <c r="S88" s="82"/>
-      <c r="T88" s="82"/>
-      <c r="U88" s="82"/>
-      <c r="V88" s="82"/>
+      <c r="B88" s="95"/>
+      <c r="C88" s="95"/>
+      <c r="D88" s="95"/>
+      <c r="E88" s="95"/>
+      <c r="F88" s="95"/>
+      <c r="G88" s="95"/>
+      <c r="H88" s="95"/>
+      <c r="I88" s="95"/>
+      <c r="J88" s="95"/>
+      <c r="K88" s="95"/>
+      <c r="L88" s="95"/>
+      <c r="M88" s="95"/>
+      <c r="N88" s="95"/>
+      <c r="O88" s="95"/>
+      <c r="P88" s="95"/>
+      <c r="Q88" s="95"/>
+      <c r="R88" s="95"/>
+      <c r="S88" s="95"/>
+      <c r="T88" s="95"/>
+      <c r="U88" s="95"/>
+      <c r="V88" s="95"/>
       <c r="W88" s="79"/>
       <c r="X88" s="79"/>
       <c r="Y88" s="79"/>
@@ -85124,30 +85089,30 @@
       <c r="AM88" s="7"/>
     </row>
     <row r="89" spans="1:39" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A89" s="85" t="s">
+      <c r="A89" s="84" t="s">
         <v>997</v>
       </c>
-      <c r="B89" s="85"/>
-      <c r="C89" s="85"/>
-      <c r="D89" s="85"/>
-      <c r="E89" s="85"/>
-      <c r="F89" s="85"/>
-      <c r="G89" s="85"/>
-      <c r="H89" s="85"/>
-      <c r="I89" s="85"/>
-      <c r="J89" s="85"/>
-      <c r="K89" s="85"/>
-      <c r="L89" s="85"/>
-      <c r="M89" s="85"/>
-      <c r="N89" s="85"/>
-      <c r="O89" s="85"/>
-      <c r="P89" s="85"/>
-      <c r="Q89" s="85"/>
-      <c r="R89" s="85"/>
-      <c r="S89" s="85"/>
-      <c r="T89" s="85"/>
-      <c r="U89" s="85"/>
-      <c r="V89" s="85"/>
+      <c r="B89" s="84"/>
+      <c r="C89" s="84"/>
+      <c r="D89" s="84"/>
+      <c r="E89" s="84"/>
+      <c r="F89" s="84"/>
+      <c r="G89" s="84"/>
+      <c r="H89" s="84"/>
+      <c r="I89" s="84"/>
+      <c r="J89" s="84"/>
+      <c r="K89" s="84"/>
+      <c r="L89" s="84"/>
+      <c r="M89" s="84"/>
+      <c r="N89" s="84"/>
+      <c r="O89" s="84"/>
+      <c r="P89" s="84"/>
+      <c r="Q89" s="84"/>
+      <c r="R89" s="84"/>
+      <c r="S89" s="84"/>
+      <c r="T89" s="84"/>
+      <c r="U89" s="84"/>
+      <c r="V89" s="84"/>
       <c r="W89" s="79"/>
       <c r="X89" s="79"/>
       <c r="Y89" s="79"/>
@@ -85167,30 +85132,30 @@
       <c r="AM89" s="7"/>
     </row>
     <row r="90" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A90" s="85" t="s">
+      <c r="A90" s="84" t="s">
         <v>1609</v>
       </c>
-      <c r="B90" s="85"/>
-      <c r="C90" s="85"/>
-      <c r="D90" s="85"/>
-      <c r="E90" s="85"/>
-      <c r="F90" s="85"/>
-      <c r="G90" s="85"/>
-      <c r="H90" s="85"/>
-      <c r="I90" s="85"/>
-      <c r="J90" s="85"/>
-      <c r="K90" s="85"/>
-      <c r="L90" s="85"/>
-      <c r="M90" s="85"/>
-      <c r="N90" s="85"/>
-      <c r="O90" s="85"/>
-      <c r="P90" s="85"/>
-      <c r="Q90" s="85"/>
-      <c r="R90" s="85"/>
-      <c r="S90" s="85"/>
-      <c r="T90" s="85"/>
-      <c r="U90" s="85"/>
-      <c r="V90" s="85"/>
+      <c r="B90" s="84"/>
+      <c r="C90" s="84"/>
+      <c r="D90" s="84"/>
+      <c r="E90" s="84"/>
+      <c r="F90" s="84"/>
+      <c r="G90" s="84"/>
+      <c r="H90" s="84"/>
+      <c r="I90" s="84"/>
+      <c r="J90" s="84"/>
+      <c r="K90" s="84"/>
+      <c r="L90" s="84"/>
+      <c r="M90" s="84"/>
+      <c r="N90" s="84"/>
+      <c r="O90" s="84"/>
+      <c r="P90" s="84"/>
+      <c r="Q90" s="84"/>
+      <c r="R90" s="84"/>
+      <c r="S90" s="84"/>
+      <c r="T90" s="84"/>
+      <c r="U90" s="84"/>
+      <c r="V90" s="84"/>
       <c r="W90" s="79"/>
       <c r="X90" s="79"/>
       <c r="Y90" s="79"/>
@@ -85210,30 +85175,30 @@
       <c r="AM90" s="7"/>
     </row>
     <row r="91" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A91" s="82" t="s">
+      <c r="A91" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B91" s="82"/>
-      <c r="C91" s="82"/>
-      <c r="D91" s="82"/>
-      <c r="E91" s="82"/>
-      <c r="F91" s="82"/>
-      <c r="G91" s="82"/>
-      <c r="H91" s="82"/>
-      <c r="I91" s="82"/>
-      <c r="J91" s="82"/>
-      <c r="K91" s="82"/>
-      <c r="L91" s="82"/>
-      <c r="M91" s="82"/>
-      <c r="N91" s="82"/>
-      <c r="O91" s="82"/>
-      <c r="P91" s="82"/>
-      <c r="Q91" s="82"/>
-      <c r="R91" s="82"/>
-      <c r="S91" s="82"/>
-      <c r="T91" s="82"/>
-      <c r="U91" s="82"/>
-      <c r="V91" s="82"/>
+      <c r="B91" s="95"/>
+      <c r="C91" s="95"/>
+      <c r="D91" s="95"/>
+      <c r="E91" s="95"/>
+      <c r="F91" s="95"/>
+      <c r="G91" s="95"/>
+      <c r="H91" s="95"/>
+      <c r="I91" s="95"/>
+      <c r="J91" s="95"/>
+      <c r="K91" s="95"/>
+      <c r="L91" s="95"/>
+      <c r="M91" s="95"/>
+      <c r="N91" s="95"/>
+      <c r="O91" s="95"/>
+      <c r="P91" s="95"/>
+      <c r="Q91" s="95"/>
+      <c r="R91" s="95"/>
+      <c r="S91" s="95"/>
+      <c r="T91" s="95"/>
+      <c r="U91" s="95"/>
+      <c r="V91" s="95"/>
       <c r="W91" s="79"/>
       <c r="X91" s="79"/>
       <c r="Y91" s="79"/>
@@ -85253,30 +85218,30 @@
       <c r="AM91" s="7"/>
     </row>
     <row r="92" spans="1:39" s="14" customFormat="1" ht="12" customHeight="1">
-      <c r="A92" s="86" t="s">
+      <c r="A92" s="96" t="s">
         <v>998</v>
       </c>
-      <c r="B92" s="86"/>
-      <c r="C92" s="86"/>
-      <c r="D92" s="86"/>
-      <c r="E92" s="86"/>
-      <c r="F92" s="86"/>
-      <c r="G92" s="86"/>
-      <c r="H92" s="86"/>
-      <c r="I92" s="86"/>
-      <c r="J92" s="86"/>
-      <c r="K92" s="86"/>
-      <c r="L92" s="86"/>
-      <c r="M92" s="86"/>
-      <c r="N92" s="86"/>
-      <c r="O92" s="86"/>
-      <c r="P92" s="86"/>
-      <c r="Q92" s="86"/>
-      <c r="R92" s="86"/>
-      <c r="S92" s="86"/>
-      <c r="T92" s="86"/>
-      <c r="U92" s="86"/>
-      <c r="V92" s="86"/>
+      <c r="B92" s="96"/>
+      <c r="C92" s="96"/>
+      <c r="D92" s="96"/>
+      <c r="E92" s="96"/>
+      <c r="F92" s="96"/>
+      <c r="G92" s="96"/>
+      <c r="H92" s="96"/>
+      <c r="I92" s="96"/>
+      <c r="J92" s="96"/>
+      <c r="K92" s="96"/>
+      <c r="L92" s="96"/>
+      <c r="M92" s="96"/>
+      <c r="N92" s="96"/>
+      <c r="O92" s="96"/>
+      <c r="P92" s="96"/>
+      <c r="Q92" s="96"/>
+      <c r="R92" s="96"/>
+      <c r="S92" s="96"/>
+      <c r="T92" s="96"/>
+      <c r="U92" s="96"/>
+      <c r="V92" s="96"/>
       <c r="W92" s="79"/>
       <c r="X92" s="79"/>
       <c r="Y92" s="79"/>
@@ -85296,30 +85261,30 @@
       <c r="AM92" s="7"/>
     </row>
     <row r="93" spans="1:39" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A93" s="85" t="s">
+      <c r="A93" s="84" t="s">
         <v>1610</v>
       </c>
-      <c r="B93" s="85"/>
-      <c r="C93" s="85"/>
-      <c r="D93" s="85"/>
-      <c r="E93" s="85"/>
-      <c r="F93" s="85"/>
-      <c r="G93" s="85"/>
-      <c r="H93" s="85"/>
-      <c r="I93" s="85"/>
-      <c r="J93" s="85"/>
-      <c r="K93" s="85"/>
-      <c r="L93" s="85"/>
-      <c r="M93" s="85"/>
-      <c r="N93" s="85"/>
-      <c r="O93" s="85"/>
-      <c r="P93" s="85"/>
-      <c r="Q93" s="85"/>
-      <c r="R93" s="85"/>
-      <c r="S93" s="85"/>
-      <c r="T93" s="85"/>
-      <c r="U93" s="85"/>
-      <c r="V93" s="85"/>
+      <c r="B93" s="84"/>
+      <c r="C93" s="84"/>
+      <c r="D93" s="84"/>
+      <c r="E93" s="84"/>
+      <c r="F93" s="84"/>
+      <c r="G93" s="84"/>
+      <c r="H93" s="84"/>
+      <c r="I93" s="84"/>
+      <c r="J93" s="84"/>
+      <c r="K93" s="84"/>
+      <c r="L93" s="84"/>
+      <c r="M93" s="84"/>
+      <c r="N93" s="84"/>
+      <c r="O93" s="84"/>
+      <c r="P93" s="84"/>
+      <c r="Q93" s="84"/>
+      <c r="R93" s="84"/>
+      <c r="S93" s="84"/>
+      <c r="T93" s="84"/>
+      <c r="U93" s="84"/>
+      <c r="V93" s="84"/>
       <c r="W93" s="79"/>
       <c r="X93" s="79"/>
       <c r="Y93" s="79"/>
@@ -85339,30 +85304,30 @@
       <c r="AM93" s="7"/>
     </row>
     <row r="94" spans="1:39" s="14" customFormat="1" ht="12" customHeight="1">
-      <c r="A94" s="83" t="s">
+      <c r="A94" s="92" t="s">
         <v>1611</v>
       </c>
-      <c r="B94" s="83"/>
-      <c r="C94" s="83"/>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
-      <c r="F94" s="83"/>
-      <c r="G94" s="83"/>
-      <c r="H94" s="83"/>
-      <c r="I94" s="83"/>
-      <c r="J94" s="83"/>
-      <c r="K94" s="83"/>
-      <c r="L94" s="83"/>
-      <c r="M94" s="83"/>
-      <c r="N94" s="83"/>
-      <c r="O94" s="83"/>
-      <c r="P94" s="83"/>
-      <c r="Q94" s="83"/>
-      <c r="R94" s="83"/>
-      <c r="S94" s="83"/>
-      <c r="T94" s="83"/>
-      <c r="U94" s="83"/>
-      <c r="V94" s="83"/>
+      <c r="B94" s="92"/>
+      <c r="C94" s="92"/>
+      <c r="D94" s="92"/>
+      <c r="E94" s="92"/>
+      <c r="F94" s="92"/>
+      <c r="G94" s="92"/>
+      <c r="H94" s="92"/>
+      <c r="I94" s="92"/>
+      <c r="J94" s="92"/>
+      <c r="K94" s="92"/>
+      <c r="L94" s="92"/>
+      <c r="M94" s="92"/>
+      <c r="N94" s="92"/>
+      <c r="O94" s="92"/>
+      <c r="P94" s="92"/>
+      <c r="Q94" s="92"/>
+      <c r="R94" s="92"/>
+      <c r="S94" s="92"/>
+      <c r="T94" s="92"/>
+      <c r="U94" s="92"/>
+      <c r="V94" s="92"/>
       <c r="W94" s="22"/>
       <c r="X94" s="22"/>
       <c r="Y94" s="22"/>
@@ -85382,30 +85347,30 @@
       <c r="AM94" s="7"/>
     </row>
     <row r="95" spans="1:39" s="15" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A95" s="82" t="s">
+      <c r="A95" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="B95" s="82"/>
-      <c r="C95" s="82"/>
-      <c r="D95" s="82"/>
-      <c r="E95" s="82"/>
-      <c r="F95" s="82"/>
-      <c r="G95" s="82"/>
-      <c r="H95" s="82"/>
-      <c r="I95" s="82"/>
-      <c r="J95" s="82"/>
-      <c r="K95" s="82"/>
-      <c r="L95" s="82"/>
-      <c r="M95" s="82"/>
-      <c r="N95" s="82"/>
-      <c r="O95" s="82"/>
-      <c r="P95" s="82"/>
-      <c r="Q95" s="82"/>
-      <c r="R95" s="82"/>
-      <c r="S95" s="82"/>
-      <c r="T95" s="82"/>
-      <c r="U95" s="82"/>
-      <c r="V95" s="82"/>
+      <c r="B95" s="95"/>
+      <c r="C95" s="95"/>
+      <c r="D95" s="95"/>
+      <c r="E95" s="95"/>
+      <c r="F95" s="95"/>
+      <c r="G95" s="95"/>
+      <c r="H95" s="95"/>
+      <c r="I95" s="95"/>
+      <c r="J95" s="95"/>
+      <c r="K95" s="95"/>
+      <c r="L95" s="95"/>
+      <c r="M95" s="95"/>
+      <c r="N95" s="95"/>
+      <c r="O95" s="95"/>
+      <c r="P95" s="95"/>
+      <c r="Q95" s="95"/>
+      <c r="R95" s="95"/>
+      <c r="S95" s="95"/>
+      <c r="T95" s="95"/>
+      <c r="U95" s="95"/>
+      <c r="V95" s="95"/>
       <c r="W95" s="79"/>
       <c r="X95" s="79"/>
       <c r="Y95" s="79"/>
@@ -85425,30 +85390,30 @@
       <c r="AM95" s="7"/>
     </row>
     <row r="96" spans="1:39" s="16" customFormat="1">
-      <c r="A96" s="84" t="s">
+      <c r="A96" s="97" t="s">
         <v>1612</v>
       </c>
-      <c r="B96" s="84"/>
-      <c r="C96" s="84"/>
-      <c r="D96" s="84"/>
-      <c r="E96" s="84"/>
-      <c r="F96" s="84"/>
-      <c r="G96" s="84"/>
-      <c r="H96" s="84"/>
-      <c r="I96" s="84"/>
-      <c r="J96" s="84"/>
-      <c r="K96" s="84"/>
-      <c r="L96" s="84"/>
-      <c r="M96" s="84"/>
-      <c r="N96" s="84"/>
-      <c r="O96" s="84"/>
-      <c r="P96" s="84"/>
-      <c r="Q96" s="84"/>
-      <c r="R96" s="84"/>
-      <c r="S96" s="84"/>
-      <c r="T96" s="84"/>
-      <c r="U96" s="84"/>
-      <c r="V96" s="84"/>
+      <c r="B96" s="97"/>
+      <c r="C96" s="97"/>
+      <c r="D96" s="97"/>
+      <c r="E96" s="97"/>
+      <c r="F96" s="97"/>
+      <c r="G96" s="97"/>
+      <c r="H96" s="97"/>
+      <c r="I96" s="97"/>
+      <c r="J96" s="97"/>
+      <c r="K96" s="97"/>
+      <c r="L96" s="97"/>
+      <c r="M96" s="97"/>
+      <c r="N96" s="97"/>
+      <c r="O96" s="97"/>
+      <c r="P96" s="97"/>
+      <c r="Q96" s="97"/>
+      <c r="R96" s="97"/>
+      <c r="S96" s="97"/>
+      <c r="T96" s="97"/>
+      <c r="U96" s="97"/>
+      <c r="V96" s="97"/>
       <c r="W96" s="79"/>
       <c r="X96" s="79"/>
       <c r="Y96" s="79"/>
@@ -85469,6 +85434,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A87:V87"/>
+    <mergeCell ref="A88:V88"/>
+    <mergeCell ref="A94:V94"/>
+    <mergeCell ref="A95:V95"/>
+    <mergeCell ref="A96:V96"/>
+    <mergeCell ref="A89:V89"/>
+    <mergeCell ref="A90:V90"/>
+    <mergeCell ref="A91:V91"/>
+    <mergeCell ref="A92:V92"/>
+    <mergeCell ref="A93:V93"/>
+    <mergeCell ref="A51:V51"/>
+    <mergeCell ref="A84:V84"/>
+    <mergeCell ref="A85:V85"/>
+    <mergeCell ref="A86:V86"/>
+    <mergeCell ref="A80:V80"/>
+    <mergeCell ref="A81:V81"/>
+    <mergeCell ref="A82:V82"/>
+    <mergeCell ref="A83:V83"/>
+    <mergeCell ref="A75:V75"/>
+    <mergeCell ref="A76:V76"/>
+    <mergeCell ref="A77:V77"/>
+    <mergeCell ref="A78:V78"/>
+    <mergeCell ref="A79:V79"/>
+    <mergeCell ref="A70:V70"/>
+    <mergeCell ref="A71:V71"/>
+    <mergeCell ref="A46:V46"/>
+    <mergeCell ref="A47:V47"/>
+    <mergeCell ref="A48:V48"/>
+    <mergeCell ref="A49:V49"/>
+    <mergeCell ref="A50:V50"/>
+    <mergeCell ref="A72:V72"/>
+    <mergeCell ref="A73:V73"/>
+    <mergeCell ref="A74:V74"/>
+    <mergeCell ref="A65:V65"/>
+    <mergeCell ref="A66:V66"/>
+    <mergeCell ref="A67:V67"/>
+    <mergeCell ref="A68:V68"/>
+    <mergeCell ref="A69:V69"/>
+    <mergeCell ref="A60:V60"/>
+    <mergeCell ref="A61:V61"/>
+    <mergeCell ref="A62:V62"/>
+    <mergeCell ref="A63:V63"/>
+    <mergeCell ref="A64:V64"/>
+    <mergeCell ref="A55:V55"/>
+    <mergeCell ref="A56:V56"/>
+    <mergeCell ref="A57:V57"/>
+    <mergeCell ref="A58:V58"/>
+    <mergeCell ref="A59:V59"/>
     <mergeCell ref="A52:V52"/>
     <mergeCell ref="A53:V53"/>
     <mergeCell ref="A54:V54"/>
@@ -85484,55 +85497,7 @@
     <mergeCell ref="A42:V42"/>
     <mergeCell ref="A43:V43"/>
     <mergeCell ref="A44:V44"/>
-    <mergeCell ref="A55:V55"/>
-    <mergeCell ref="A56:V56"/>
-    <mergeCell ref="A57:V57"/>
-    <mergeCell ref="A58:V58"/>
-    <mergeCell ref="A59:V59"/>
-    <mergeCell ref="A60:V60"/>
-    <mergeCell ref="A61:V61"/>
-    <mergeCell ref="A62:V62"/>
-    <mergeCell ref="A63:V63"/>
-    <mergeCell ref="A64:V64"/>
-    <mergeCell ref="A72:V72"/>
-    <mergeCell ref="A73:V73"/>
-    <mergeCell ref="A74:V74"/>
-    <mergeCell ref="A65:V65"/>
-    <mergeCell ref="A66:V66"/>
-    <mergeCell ref="A67:V67"/>
-    <mergeCell ref="A68:V68"/>
-    <mergeCell ref="A69:V69"/>
     <mergeCell ref="A45:V45"/>
-    <mergeCell ref="A46:V46"/>
-    <mergeCell ref="A47:V47"/>
-    <mergeCell ref="A48:V48"/>
-    <mergeCell ref="A49:V49"/>
-    <mergeCell ref="A50:V50"/>
-    <mergeCell ref="A51:V51"/>
-    <mergeCell ref="A84:V84"/>
-    <mergeCell ref="A85:V85"/>
-    <mergeCell ref="A86:V86"/>
-    <mergeCell ref="A80:V80"/>
-    <mergeCell ref="A81:V81"/>
-    <mergeCell ref="A82:V82"/>
-    <mergeCell ref="A83:V83"/>
-    <mergeCell ref="A75:V75"/>
-    <mergeCell ref="A76:V76"/>
-    <mergeCell ref="A77:V77"/>
-    <mergeCell ref="A78:V78"/>
-    <mergeCell ref="A79:V79"/>
-    <mergeCell ref="A70:V70"/>
-    <mergeCell ref="A71:V71"/>
-    <mergeCell ref="A87:V87"/>
-    <mergeCell ref="A88:V88"/>
-    <mergeCell ref="A94:V94"/>
-    <mergeCell ref="A95:V95"/>
-    <mergeCell ref="A96:V96"/>
-    <mergeCell ref="A89:V89"/>
-    <mergeCell ref="A90:V90"/>
-    <mergeCell ref="A91:V91"/>
-    <mergeCell ref="A92:V92"/>
-    <mergeCell ref="A93:V93"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AN32">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="false">

</xml_diff>